<commit_message>
0.0.7: Kotlin preferred defautl value is implemented. Class with generic type now able to be defined.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F16AA7-304F-884B-919D-20C216A640E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEEA544-AFC6-3448-B77F-0051A8918BF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9180" yWindow="2100" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
   <si>
     <t>クラス名</t>
   </si>
@@ -442,6 +442,29 @@
     <rPh sb="4" eb="7">
       <t xml:space="preserve">ソウショウガタ </t>
     </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>デフォルト(Kt)</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"kotlin優先"</t>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">ユウセｎ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"デフォルト2"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>arrayListOf()</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>new Array&lt;SimpleSample&gt;</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -539,7 +562,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -871,19 +894,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -1016,38 +1026,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1055,7 +1039,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1119,9 +1103,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1130,21 +1112,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1152,22 +1133,22 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="33" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1186,23 +1167,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1242,6 +1212,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1653,46 +1633,50 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="6" width="23.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.83203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="28" style="1" customWidth="1"/>
-    <col min="14" max="14" width="33.33203125" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="1"/>
+    <col min="2" max="7" width="23.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.83203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="28" style="1" customWidth="1"/>
+    <col min="15" max="15" width="33.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19">
+    <row r="1" spans="1:14" ht="19">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="4" spans="1:14">
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1701,12 +1685,13 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="80"/>
+      <c r="G5" s="86"/>
       <c r="H5" s="38"/>
       <c r="I5" s="38"/>
       <c r="J5" s="38"/>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="K5" s="38"/>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1717,13 +1702,14 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="81"/>
+      <c r="G6" s="86"/>
       <c r="H6" s="38"/>
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
-      <c r="K6" s="39"/>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="K6" s="38"/>
+      <c r="L6" s="39"/>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1734,13 +1720,14 @@
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="81"/>
+      <c r="G7" s="86"/>
       <c r="H7" s="38"/>
       <c r="I7" s="38"/>
       <c r="J7" s="38"/>
-      <c r="K7" s="39"/>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="K7" s="38"/>
+      <c r="L7" s="39"/>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1751,13 +1738,14 @@
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="81"/>
+      <c r="G8" s="86"/>
       <c r="H8" s="38"/>
       <c r="I8" s="38"/>
       <c r="J8" s="38"/>
-      <c r="K8" s="39"/>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="K8" s="38"/>
+      <c r="L8" s="39"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="3" t="s">
         <v>71</v>
       </c>
@@ -1768,51 +1756,54 @@
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="81" t="s">
+      <c r="G9" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="H9" s="38"/>
+      <c r="H9" s="41"/>
       <c r="I9" s="38"/>
       <c r="J9" s="38"/>
-      <c r="K9" s="39"/>
-    </row>
-    <row r="10" spans="1:13" ht="45">
+      <c r="K9" s="38"/>
+      <c r="L9" s="39"/>
+    </row>
+    <row r="10" spans="1:14" ht="45">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="74" t="s">
         <v>67</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="81"/>
+      <c r="G10" s="86"/>
       <c r="H10" s="38"/>
       <c r="I10" s="38"/>
       <c r="J10" s="38"/>
-      <c r="K10" s="39"/>
-    </row>
-    <row r="11" spans="1:13" ht="29" customHeight="1">
+      <c r="K10" s="38"/>
+      <c r="L10" s="39"/>
+    </row>
+    <row r="11" spans="1:14" ht="29" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="86" t="s">
+      <c r="C11" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="87"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="38"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
       <c r="L11" s="38"/>
       <c r="M11" s="38"/>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11" s="38"/>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -1823,35 +1814,37 @@
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="81"/>
+      <c r="G12" s="86"/>
       <c r="H12" s="38"/>
       <c r="I12" s="38"/>
       <c r="J12" s="38"/>
       <c r="K12" s="38"/>
       <c r="L12" s="38"/>
       <c r="M12" s="38"/>
-    </row>
-    <row r="13" spans="1:13" s="33" customFormat="1">
-      <c r="A13" s="66" t="s">
+      <c r="N12" s="38"/>
+    </row>
+    <row r="13" spans="1:14" s="33" customFormat="1">
+      <c r="A13" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="67"/>
-      <c r="C13" s="68"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="65"/>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13" s="70"/>
-      <c r="I13" s="70"/>
-      <c r="J13" s="73"/>
-      <c r="K13"/>
-    </row>
-    <row r="14" spans="1:13" s="33" customFormat="1">
-      <c r="A14" s="66" t="s">
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="70"/>
+      <c r="L13"/>
+    </row>
+    <row r="14" spans="1:14" s="33" customFormat="1">
+      <c r="A14" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="67"/>
-      <c r="C14" s="68" t="s">
+      <c r="B14" s="64"/>
+      <c r="C14" s="65" t="s">
         <v>45</v>
       </c>
       <c r="D14" t="s">
@@ -1859,79 +1852,84 @@
       </c>
       <c r="E14"/>
       <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="73"/>
-      <c r="K14"/>
-    </row>
-    <row r="15" spans="1:13" s="33" customFormat="1">
-      <c r="A15" s="66" t="s">
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="70"/>
+      <c r="L14"/>
+    </row>
+    <row r="15" spans="1:14" s="33" customFormat="1">
+      <c r="A15" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="67"/>
-      <c r="C15" s="68"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="65"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="73"/>
-      <c r="K15"/>
-    </row>
-    <row r="16" spans="1:13" s="33" customFormat="1">
-      <c r="A16" s="66" t="s">
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="70"/>
+      <c r="L15"/>
+    </row>
+    <row r="16" spans="1:14" s="33" customFormat="1">
+      <c r="A16" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="67"/>
-      <c r="C16" s="68" t="s">
+      <c r="B16" s="64"/>
+      <c r="C16" s="65" t="s">
         <v>45</v>
       </c>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="70"/>
-      <c r="J16" s="73"/>
-      <c r="K16"/>
-    </row>
-    <row r="17" spans="1:15" s="33" customFormat="1">
-      <c r="A17" s="66" t="s">
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="70"/>
+      <c r="L16"/>
+    </row>
+    <row r="17" spans="1:16" s="33" customFormat="1">
+      <c r="A17" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="67"/>
-      <c r="C17" s="68" t="s">
+      <c r="B17" s="64"/>
+      <c r="C17" s="65" t="s">
         <v>45</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="73"/>
-      <c r="K17"/>
-    </row>
-    <row r="18" spans="1:15" s="33" customFormat="1">
-      <c r="A18" s="66" t="s">
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="70"/>
+      <c r="L17"/>
+    </row>
+    <row r="18" spans="1:16" s="33" customFormat="1">
+      <c r="A18" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="68" t="s">
+      <c r="B18" s="64"/>
+      <c r="C18" s="65" t="s">
         <v>45</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="73"/>
-      <c r="K18"/>
-    </row>
-    <row r="19" spans="1:15" s="41" customFormat="1">
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="70"/>
+      <c r="L18"/>
+    </row>
+    <row r="19" spans="1:16" s="41" customFormat="1">
       <c r="A19" s="38"/>
       <c r="B19" s="40"/>
       <c r="C19" s="38"/>
@@ -1945,8 +1943,9 @@
       <c r="K19" s="38"/>
       <c r="L19" s="38"/>
       <c r="M19" s="38"/>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="N19" s="38"/>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="31" t="s">
         <v>16</v>
       </c>
@@ -1954,18 +1953,19 @@
       <c r="C20" s="32"/>
       <c r="D20" s="32"/>
       <c r="E20" s="32"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="33"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
       <c r="M20" s="33"/>
       <c r="N20" s="33"/>
       <c r="O20" s="33"/>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="P20" s="33"/>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="34" t="s">
         <v>0</v>
       </c>
@@ -1973,18 +1973,19 @@
       <c r="C21" s="36"/>
       <c r="D21" s="36"/>
       <c r="E21" s="36"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="71"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="71"/>
-      <c r="K21" s="71"/>
-      <c r="L21" s="33"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="89"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="68"/>
+      <c r="K21" s="68"/>
+      <c r="L21" s="68"/>
       <c r="M21" s="33"/>
       <c r="N21" s="33"/>
       <c r="O21" s="33"/>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="P21" s="33"/>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
@@ -1992,14 +1993,15 @@
       <c r="C22" s="10"/>
       <c r="D22" s="37"/>
       <c r="E22" s="37"/>
-      <c r="F22" s="76"/>
-      <c r="G22" s="38"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="90"/>
       <c r="H22" s="38"/>
       <c r="I22" s="38"/>
       <c r="J22" s="38"/>
-      <c r="K22" s="39"/>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="K22" s="38"/>
+      <c r="L22" s="39"/>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -2007,14 +2009,15 @@
       <c r="C23" s="7"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="38"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="90"/>
       <c r="H23" s="38"/>
       <c r="I23" s="38"/>
       <c r="J23" s="38"/>
-      <c r="K23" s="39"/>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="K23" s="38"/>
+      <c r="L23" s="39"/>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="38"/>
       <c r="B24" s="40"/>
       <c r="C24" s="38"/>
@@ -2025,9 +2028,10 @@
       <c r="H24" s="38"/>
       <c r="I24" s="38"/>
       <c r="J24" s="38"/>
-      <c r="K24" s="39"/>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="K24" s="38"/>
+      <c r="L24" s="39"/>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="31" t="s">
         <v>55</v>
       </c>
@@ -2036,89 +2040,94 @@
       <c r="D25" s="32"/>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="47"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
-      <c r="O25" s="47"/>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="51" t="s">
+      <c r="G25" s="88"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="45"/>
+      <c r="N25" s="45"/>
+      <c r="O25" s="45"/>
+      <c r="P25" s="45"/>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="71"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="49"/>
-      <c r="N26" s="49"/>
-      <c r="O26" s="39"/>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="55"/>
-      <c r="B27" s="50"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="89"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="68"/>
+      <c r="L26" s="68"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="39"/>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="52"/>
+      <c r="B27" s="48"/>
       <c r="C27" s="42"/>
       <c r="D27" s="42"/>
       <c r="E27" s="42"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="72"/>
-      <c r="H27" s="72"/>
-      <c r="I27" s="72"/>
-      <c r="J27" s="72"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="40"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="91"/>
+      <c r="H27" s="69"/>
+      <c r="I27" s="69"/>
+      <c r="J27" s="69"/>
+      <c r="K27" s="69"/>
+      <c r="L27" s="38"/>
       <c r="M27" s="40"/>
       <c r="N27" s="40"/>
-      <c r="O27" s="39"/>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="55"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="72"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="72"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="40"/>
+      <c r="O27" s="40"/>
+      <c r="P27" s="39"/>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="52"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="91"/>
+      <c r="H28" s="69"/>
+      <c r="I28" s="69"/>
+      <c r="J28" s="69"/>
+      <c r="K28" s="69"/>
+      <c r="L28" s="38"/>
       <c r="M28" s="40"/>
       <c r="N28" s="40"/>
-      <c r="O28" s="39"/>
-    </row>
-    <row r="29" spans="1:15">
-      <c r="A29" s="56"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="72"/>
-      <c r="I29" s="72"/>
-      <c r="J29" s="72"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="40"/>
+      <c r="O28" s="40"/>
+      <c r="P28" s="39"/>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="53"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="91"/>
+      <c r="H29" s="69"/>
+      <c r="I29" s="69"/>
+      <c r="J29" s="69"/>
+      <c r="K29" s="69"/>
+      <c r="L29" s="38"/>
       <c r="M29" s="40"/>
       <c r="N29" s="40"/>
-      <c r="O29" s="39"/>
-    </row>
-    <row r="30" spans="1:15" s="41" customFormat="1">
+      <c r="O29" s="40"/>
+      <c r="P29" s="39"/>
+    </row>
+    <row r="30" spans="1:16" s="41" customFormat="1">
       <c r="A30" s="38"/>
       <c r="B30" s="40"/>
       <c r="C30" s="38"/>
@@ -2132,8 +2141,9 @@
       <c r="K30" s="38"/>
       <c r="L30" s="38"/>
       <c r="M30" s="38"/>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="N30" s="38"/>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="31" t="s">
         <v>31</v>
       </c>
@@ -2142,93 +2152,98 @@
       <c r="D31" s="32"/>
       <c r="E31" s="32"/>
       <c r="F31" s="32"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="47"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="47"/>
-      <c r="O31" s="47"/>
-    </row>
-    <row r="32" spans="1:15">
-      <c r="A32" s="51" t="s">
+      <c r="G31" s="88"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="45"/>
+      <c r="O31" s="45"/>
+      <c r="P31" s="45"/>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="71"/>
-      <c r="H32" s="71"/>
-      <c r="I32" s="71"/>
-      <c r="J32" s="71"/>
-      <c r="K32" s="71"/>
-      <c r="L32" s="48"/>
-      <c r="M32" s="49"/>
-      <c r="N32" s="49"/>
-      <c r="O32" s="39"/>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="A33" s="55">
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="89"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="68"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="68"/>
+      <c r="M32" s="46"/>
+      <c r="N32" s="47"/>
+      <c r="O32" s="47"/>
+      <c r="P32" s="39"/>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="52">
         <v>1</v>
       </c>
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="48" t="s">
         <v>59</v>
       </c>
       <c r="C33" s="42"/>
       <c r="D33" s="42"/>
       <c r="E33" s="42"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="72"/>
-      <c r="H33" s="72"/>
-      <c r="I33" s="72"/>
-      <c r="J33" s="72"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="40"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="91"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="69"/>
+      <c r="J33" s="69"/>
+      <c r="K33" s="69"/>
+      <c r="L33" s="38"/>
       <c r="M33" s="40"/>
       <c r="N33" s="40"/>
-      <c r="O33" s="39"/>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" s="55"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="72"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="72"/>
-      <c r="K34" s="38"/>
-      <c r="L34" s="40"/>
+      <c r="O33" s="40"/>
+      <c r="P33" s="39"/>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="52"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="91"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="69"/>
+      <c r="K34" s="69"/>
+      <c r="L34" s="38"/>
       <c r="M34" s="40"/>
       <c r="N34" s="40"/>
-      <c r="O34" s="39"/>
-    </row>
-    <row r="35" spans="1:15">
-      <c r="A35" s="56"/>
-      <c r="B35" s="52"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="72"/>
-      <c r="H35" s="72"/>
-      <c r="I35" s="72"/>
-      <c r="J35" s="72"/>
-      <c r="K35" s="38"/>
-      <c r="L35" s="40"/>
+      <c r="O34" s="40"/>
+      <c r="P34" s="39"/>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" s="53"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="91"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="69"/>
+      <c r="L35" s="38"/>
       <c r="M35" s="40"/>
       <c r="N35" s="40"/>
-      <c r="O35" s="39"/>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="O35" s="40"/>
+      <c r="P35" s="39"/>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -2241,8 +2256,9 @@
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="M36" s="13"/>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" s="3" t="s">
         <v>11</v>
       </c>
@@ -2258,66 +2274,71 @@
       <c r="K37" s="14"/>
       <c r="L37" s="14"/>
       <c r="M37" s="14"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="15"/>
-    </row>
-    <row r="38" spans="1:15" ht="13.5" customHeight="1">
-      <c r="A38" s="90" t="s">
+      <c r="N37" s="14"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="15"/>
+    </row>
+    <row r="38" spans="1:16" ht="13.5" customHeight="1">
+      <c r="A38" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="90" t="s">
+      <c r="B38" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="89" t="s">
+      <c r="C38" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="89" t="s">
+      <c r="D38" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="91" t="s">
+      <c r="E38" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="F38" s="89" t="s">
+      <c r="F38" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="91" t="s">
+      <c r="G38" s="79" t="s">
+        <v>76</v>
+      </c>
+      <c r="H38" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="H38" s="91" t="s">
+      <c r="I38" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="I38" s="94" t="s">
+      <c r="J38" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="J38" s="94" t="s">
+      <c r="K38" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="K38" s="89" t="s">
+      <c r="L38" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="L38" s="89"/>
-      <c r="M38" s="16"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="9"/>
-    </row>
-    <row r="39" spans="1:15">
-      <c r="A39" s="90"/>
-      <c r="B39" s="90"/>
-      <c r="C39" s="89"/>
-      <c r="D39" s="89"/>
-      <c r="E39" s="92"/>
-      <c r="F39" s="89"/>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="95"/>
-      <c r="J39" s="95"/>
-      <c r="K39" s="89"/>
-      <c r="L39" s="89"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="30"/>
-      <c r="O39" s="15"/>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="M38" s="79"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="9"/>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" s="80"/>
+      <c r="B39" s="80"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="79"/>
+      <c r="E39" s="82"/>
+      <c r="F39" s="79"/>
+      <c r="G39" s="79"/>
+      <c r="H39" s="83"/>
+      <c r="I39" s="83"/>
+      <c r="J39" s="85"/>
+      <c r="K39" s="85"/>
+      <c r="L39" s="79"/>
+      <c r="M39" s="79"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="30"/>
+      <c r="P39" s="15"/>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" s="19">
         <v>1</v>
       </c>
@@ -2334,23 +2355,26 @@
       <c r="F40" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G40" s="21"/>
-      <c r="H40" s="78"/>
-      <c r="I40" s="78" t="s">
+      <c r="G40" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="H40" s="21"/>
+      <c r="I40" s="71"/>
+      <c r="J40" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="J40" s="78" t="s">
+      <c r="K40" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="K40" s="21" t="s">
+      <c r="L40" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="L40" s="22"/>
       <c r="M40" s="22"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="15"/>
-    </row>
-    <row r="41" spans="1:15" ht="60">
+      <c r="N40" s="22"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="15"/>
+    </row>
+    <row r="41" spans="1:16" ht="60">
       <c r="A41" s="19">
         <f>A40+1</f>
         <v>2</v>
@@ -2362,23 +2386,24 @@
         <v>53</v>
       </c>
       <c r="D41" s="21"/>
-      <c r="E41" s="85" t="s">
+      <c r="E41" s="75" t="s">
         <v>68</v>
       </c>
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
-      <c r="H41" s="78"/>
-      <c r="I41" s="78"/>
-      <c r="J41" s="78" t="s">
+      <c r="H41" s="21"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="71"/>
+      <c r="K41" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="K41" s="21"/>
-      <c r="L41" s="22"/>
+      <c r="L41" s="21"/>
       <c r="M41" s="22"/>
-      <c r="N41" s="29"/>
-      <c r="O41" s="15"/>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="N41" s="22"/>
+      <c r="O41" s="29"/>
+      <c r="P41" s="15"/>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42" s="19">
         <f t="shared" ref="A42:A44" si="0">A41+1</f>
         <v>3</v>
@@ -2393,22 +2418,27 @@
         <v>20</v>
       </c>
       <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="78" t="s">
+      <c r="F42" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="G42" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="H42" s="21"/>
+      <c r="I42" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="I42" s="78"/>
-      <c r="J42" s="78"/>
-      <c r="K42" s="21" t="s">
+      <c r="J42" s="71"/>
+      <c r="K42" s="71"/>
+      <c r="L42" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="L42" s="22"/>
       <c r="M42" s="22"/>
-      <c r="N42" s="23"/>
-      <c r="O42" s="15"/>
-    </row>
-    <row r="43" spans="1:15" ht="30">
+      <c r="N42" s="22"/>
+      <c r="O42" s="23"/>
+      <c r="P42" s="15"/>
+    </row>
+    <row r="43" spans="1:16" ht="30">
       <c r="A43" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2420,23 +2450,26 @@
         <v>25</v>
       </c>
       <c r="D43" s="21"/>
-      <c r="E43" s="85" t="s">
+      <c r="E43" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="F43" s="21"/>
+      <c r="F43" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="G43" s="21"/>
-      <c r="H43" s="78"/>
-      <c r="I43" s="78"/>
-      <c r="J43" s="78"/>
-      <c r="K43" s="21" t="s">
+      <c r="H43" s="21"/>
+      <c r="I43" s="71"/>
+      <c r="J43" s="71"/>
+      <c r="K43" s="71"/>
+      <c r="L43" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="L43" s="22"/>
       <c r="M43" s="22"/>
-      <c r="N43" s="23"/>
-      <c r="O43" s="15"/>
-    </row>
-    <row r="44" spans="1:15" ht="15">
+      <c r="N43" s="22"/>
+      <c r="O43" s="23"/>
+      <c r="P43" s="15"/>
+    </row>
+    <row r="44" spans="1:16" ht="15">
       <c r="A44" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2448,23 +2481,24 @@
         <v>20</v>
       </c>
       <c r="D44" s="21"/>
-      <c r="E44" s="83" t="s">
+      <c r="E44" s="73" t="s">
         <v>69</v>
       </c>
       <c r="F44" s="21"/>
       <c r="G44" s="21"/>
-      <c r="H44" s="78"/>
-      <c r="I44" s="78"/>
-      <c r="J44" s="78"/>
-      <c r="K44" s="21" t="s">
+      <c r="H44" s="21"/>
+      <c r="I44" s="71"/>
+      <c r="J44" s="71"/>
+      <c r="K44" s="71"/>
+      <c r="L44" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="L44" s="22"/>
       <c r="M44" s="22"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="15"/>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="N44" s="22"/>
+      <c r="O44" s="23"/>
+      <c r="P44" s="15"/>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45" s="24">
         <v>6</v>
       </c>
@@ -2478,20 +2512,21 @@
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="79" t="s">
+      <c r="H45" s="26"/>
+      <c r="I45" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="I45" s="79"/>
-      <c r="J45" s="79"/>
-      <c r="K45" s="26" t="s">
+      <c r="J45" s="72"/>
+      <c r="K45" s="72"/>
+      <c r="L45" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="L45" s="27"/>
       <c r="M45" s="27"/>
-      <c r="N45" s="28"/>
-      <c r="O45" s="15"/>
-    </row>
-    <row r="46" spans="1:15">
+      <c r="N45" s="27"/>
+      <c r="O45" s="28"/>
+      <c r="P45" s="15"/>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46" s="24"/>
       <c r="B46" s="25"/>
       <c r="C46" s="26"/>
@@ -2499,33 +2534,35 @@
       <c r="E46" s="26"/>
       <c r="F46" s="26"/>
       <c r="G46" s="26"/>
-      <c r="H46" s="79"/>
-      <c r="I46" s="79"/>
-      <c r="J46" s="79"/>
-      <c r="K46" s="26"/>
-      <c r="L46" s="27"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="72"/>
+      <c r="J46" s="72"/>
+      <c r="K46" s="72"/>
+      <c r="L46" s="26"/>
       <c r="M46" s="27"/>
-      <c r="N46" s="28"/>
-      <c r="O46" s="15"/>
+      <c r="N46" s="27"/>
+      <c r="O46" s="28"/>
+      <c r="P46" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="C11:F11"/>
-    <mergeCell ref="K38:L39"/>
+    <mergeCell ref="L38:M39"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="F38:F39"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="E38:E39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="J38:J39"/>
     <mergeCell ref="H38:H39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="I38:I39"/>
     <mergeCell ref="G38:G39"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F62:J62" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F62:K62" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2538,7 +2575,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15 G40:G46" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15 H40:H46" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>isAbstract</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{061A2328-C320-074B-A7A0-1D5ADA23E625}">
@@ -2560,7 +2597,7 @@
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H40:J46</xm:sqref>
+          <xm:sqref>I40:K46</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2581,107 +2618,107 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="59" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="59" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="59" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" style="59" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="59" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" style="59" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="59" customWidth="1"/>
-    <col min="10" max="10" width="18.5" style="59" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="59" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="59" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="59" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" style="59" bestFit="1" customWidth="1"/>
-    <col min="15" max="260" width="8.83203125" style="59" customWidth="1"/>
-    <col min="261" max="16384" width="10.83203125" style="59"/>
+    <col min="1" max="3" width="8.83203125" style="56" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="56" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="56" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="56" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="56" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" style="56" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="56" customWidth="1"/>
+    <col min="10" max="10" width="18.5" style="56" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="56" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="56" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="56" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" style="56" bestFit="1" customWidth="1"/>
+    <col min="15" max="260" width="8.83203125" style="56" customWidth="1"/>
+    <col min="261" max="16384" width="10.83203125" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="58" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="58"/>
+      <c r="Q1" s="55"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="60" t="s">
+      <c r="F3" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="60" t="s">
+      <c r="H3" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="60" t="s">
+      <c r="L3" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="60" t="s">
+      <c r="N3" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="60" t="s">
+      <c r="P3" s="57" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="B4" s="61"/>
-      <c r="D4" s="64" t="s">
+      <c r="B4" s="58"/>
+      <c r="D4" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="H4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="L4" s="62"/>
-      <c r="N4" s="62"/>
-      <c r="P4" s="62"/>
+      <c r="H4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="P4" s="59"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="H5" s="64" t="s">
+      <c r="D5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="H5" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="64" t="s">
+      <c r="J5" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="64" t="s">
+      <c r="L5" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="64" t="s">
+      <c r="N5" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="P5" s="64" t="s">
+      <c r="P5" s="61" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="B6" s="65"/>
+      <c r="B6" s="62"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>

</xml_diff>

<commit_message>
0.0.8: FIX bug on kotlin preferred default value.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEEA544-AFC6-3448-B77F-0051A8918BF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68A0B8D-CE01-4441-81D8-BC0240D72901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9180" yWindow="2100" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
   <si>
     <t>クラス名</t>
   </si>
@@ -465,6 +465,10 @@
   </si>
   <si>
     <t>new Array&lt;SimpleSample&gt;</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>SimpleSample()</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1182,36 +1186,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1222,6 +1196,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1636,7 +1640,7 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1685,7 +1689,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="86"/>
+      <c r="G5" s="76"/>
       <c r="H5" s="38"/>
       <c r="I5" s="38"/>
       <c r="J5" s="38"/>
@@ -1702,7 +1706,7 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="86"/>
+      <c r="G6" s="76"/>
       <c r="H6" s="38"/>
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
@@ -1720,7 +1724,7 @@
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="86"/>
+      <c r="G7" s="76"/>
       <c r="H7" s="38"/>
       <c r="I7" s="38"/>
       <c r="J7" s="38"/>
@@ -1738,7 +1742,7 @@
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="86"/>
+      <c r="G8" s="76"/>
       <c r="H8" s="38"/>
       <c r="I8" s="38"/>
       <c r="J8" s="38"/>
@@ -1776,7 +1780,7 @@
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="86"/>
+      <c r="G10" s="76"/>
       <c r="H10" s="38"/>
       <c r="I10" s="38"/>
       <c r="J10" s="38"/>
@@ -1788,13 +1792,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="76" t="s">
+      <c r="C11" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="87"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="77"/>
       <c r="H11" s="66"/>
       <c r="I11" s="66"/>
       <c r="J11" s="66"/>
@@ -1814,7 +1818,7 @@
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="86"/>
+      <c r="G12" s="76"/>
       <c r="H12" s="38"/>
       <c r="I12" s="38"/>
       <c r="J12" s="38"/>
@@ -1954,7 +1958,7 @@
       <c r="D20" s="32"/>
       <c r="E20" s="32"/>
       <c r="F20" s="32"/>
-      <c r="G20" s="88"/>
+      <c r="G20" s="78"/>
       <c r="H20" s="46"/>
       <c r="I20" s="46"/>
       <c r="J20" s="46"/>
@@ -1974,7 +1978,7 @@
       <c r="D21" s="36"/>
       <c r="E21" s="36"/>
       <c r="F21" s="36"/>
-      <c r="G21" s="89"/>
+      <c r="G21" s="79"/>
       <c r="H21" s="68"/>
       <c r="I21" s="68"/>
       <c r="J21" s="68"/>
@@ -1994,7 +1998,7 @@
       <c r="D22" s="37"/>
       <c r="E22" s="37"/>
       <c r="F22" s="37"/>
-      <c r="G22" s="90"/>
+      <c r="G22" s="80"/>
       <c r="H22" s="38"/>
       <c r="I22" s="38"/>
       <c r="J22" s="38"/>
@@ -2010,7 +2014,7 @@
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
-      <c r="G23" s="90"/>
+      <c r="G23" s="80"/>
       <c r="H23" s="38"/>
       <c r="I23" s="38"/>
       <c r="J23" s="38"/>
@@ -2040,7 +2044,7 @@
       <c r="D25" s="32"/>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
-      <c r="G25" s="88"/>
+      <c r="G25" s="78"/>
       <c r="H25" s="46"/>
       <c r="I25" s="46"/>
       <c r="J25" s="46"/>
@@ -2062,7 +2066,7 @@
       <c r="D26" s="44"/>
       <c r="E26" s="44"/>
       <c r="F26" s="44"/>
-      <c r="G26" s="89"/>
+      <c r="G26" s="79"/>
       <c r="H26" s="68"/>
       <c r="I26" s="68"/>
       <c r="J26" s="68"/>
@@ -2080,7 +2084,7 @@
       <c r="D27" s="42"/>
       <c r="E27" s="42"/>
       <c r="F27" s="42"/>
-      <c r="G27" s="91"/>
+      <c r="G27" s="81"/>
       <c r="H27" s="69"/>
       <c r="I27" s="69"/>
       <c r="J27" s="69"/>
@@ -2098,7 +2102,7 @@
       <c r="D28" s="43"/>
       <c r="E28" s="43"/>
       <c r="F28" s="43"/>
-      <c r="G28" s="91"/>
+      <c r="G28" s="81"/>
       <c r="H28" s="69"/>
       <c r="I28" s="69"/>
       <c r="J28" s="69"/>
@@ -2116,7 +2120,7 @@
       <c r="D29" s="51"/>
       <c r="E29" s="51"/>
       <c r="F29" s="51"/>
-      <c r="G29" s="91"/>
+      <c r="G29" s="81"/>
       <c r="H29" s="69"/>
       <c r="I29" s="69"/>
       <c r="J29" s="69"/>
@@ -2152,7 +2156,7 @@
       <c r="D31" s="32"/>
       <c r="E31" s="32"/>
       <c r="F31" s="32"/>
-      <c r="G31" s="88"/>
+      <c r="G31" s="78"/>
       <c r="H31" s="46"/>
       <c r="I31" s="46"/>
       <c r="J31" s="46"/>
@@ -2174,7 +2178,7 @@
       <c r="D32" s="44"/>
       <c r="E32" s="44"/>
       <c r="F32" s="44"/>
-      <c r="G32" s="89"/>
+      <c r="G32" s="79"/>
       <c r="H32" s="68"/>
       <c r="I32" s="68"/>
       <c r="J32" s="68"/>
@@ -2196,7 +2200,7 @@
       <c r="D33" s="42"/>
       <c r="E33" s="42"/>
       <c r="F33" s="42"/>
-      <c r="G33" s="91"/>
+      <c r="G33" s="81"/>
       <c r="H33" s="69"/>
       <c r="I33" s="69"/>
       <c r="J33" s="69"/>
@@ -2214,7 +2218,7 @@
       <c r="D34" s="43"/>
       <c r="E34" s="43"/>
       <c r="F34" s="43"/>
-      <c r="G34" s="91"/>
+      <c r="G34" s="81"/>
       <c r="H34" s="69"/>
       <c r="I34" s="69"/>
       <c r="J34" s="69"/>
@@ -2232,7 +2236,7 @@
       <c r="D35" s="51"/>
       <c r="E35" s="51"/>
       <c r="F35" s="51"/>
-      <c r="G35" s="91"/>
+      <c r="G35" s="81"/>
       <c r="H35" s="69"/>
       <c r="I35" s="69"/>
       <c r="J35" s="69"/>
@@ -2279,61 +2283,61 @@
       <c r="P37" s="15"/>
     </row>
     <row r="38" spans="1:16" ht="13.5" customHeight="1">
-      <c r="A38" s="80" t="s">
+      <c r="A38" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="80" t="s">
+      <c r="B38" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="79" t="s">
+      <c r="C38" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="79" t="s">
+      <c r="D38" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="81" t="s">
+      <c r="E38" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="F38" s="79" t="s">
+      <c r="F38" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="79" t="s">
+      <c r="G38" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="H38" s="81" t="s">
+      <c r="H38" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="I38" s="81" t="s">
+      <c r="I38" s="87" t="s">
         <v>49</v>
       </c>
-      <c r="J38" s="84" t="s">
+      <c r="J38" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="K38" s="84" t="s">
+      <c r="K38" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="L38" s="79" t="s">
+      <c r="L38" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="M38" s="79"/>
+      <c r="M38" s="85"/>
       <c r="N38" s="16"/>
       <c r="O38" s="17"/>
       <c r="P38" s="9"/>
     </row>
     <row r="39" spans="1:16">
-      <c r="A39" s="80"/>
-      <c r="B39" s="80"/>
-      <c r="C39" s="79"/>
-      <c r="D39" s="79"/>
-      <c r="E39" s="82"/>
-      <c r="F39" s="79"/>
-      <c r="G39" s="79"/>
-      <c r="H39" s="83"/>
-      <c r="I39" s="83"/>
-      <c r="J39" s="85"/>
-      <c r="K39" s="85"/>
-      <c r="L39" s="79"/>
-      <c r="M39" s="79"/>
+      <c r="A39" s="86"/>
+      <c r="B39" s="86"/>
+      <c r="C39" s="85"/>
+      <c r="D39" s="85"/>
+      <c r="E39" s="88"/>
+      <c r="F39" s="85"/>
+      <c r="G39" s="85"/>
+      <c r="H39" s="89"/>
+      <c r="I39" s="89"/>
+      <c r="J39" s="91"/>
+      <c r="K39" s="91"/>
+      <c r="L39" s="85"/>
+      <c r="M39" s="85"/>
       <c r="N39" s="18"/>
       <c r="O39" s="30"/>
       <c r="P39" s="15"/>
@@ -2390,7 +2394,9 @@
         <v>68</v>
       </c>
       <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
+      <c r="G41" s="21">
+        <v>0</v>
+      </c>
       <c r="H41" s="21"/>
       <c r="I41" s="71"/>
       <c r="J41" s="71"/>
@@ -2485,7 +2491,9 @@
         <v>69</v>
       </c>
       <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
+      <c r="G44" s="21" t="s">
+        <v>81</v>
+      </c>
       <c r="H44" s="21"/>
       <c r="I44" s="71"/>
       <c r="J44" s="71"/>

</xml_diff>

<commit_message>
0.0.9: Adapt kotlin preferred type and annotation specifications.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68A0B8D-CE01-4441-81D8-BC0240D72901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B7331E-8C49-7C44-AD1C-52C242E7CC10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="2100" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="5380" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
   <si>
     <t>クラス名</t>
   </si>
@@ -469,6 +469,32 @@
   </si>
   <si>
     <t>SimpleSample()</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>型(Kt)</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>総称型(Kt)</t>
+    <rPh sb="0" eb="2">
+      <t>ソウショウガタ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>アノテーション(Kt)</t>
+    <rPh sb="0" eb="2">
+      <t>ソウショウガタ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ApiTelegram</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>@JsonProperty</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -566,7 +592,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -765,19 +791,6 @@
     <border>
       <left/>
       <right/>
-      <top style="hair">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
       <top style="hair">
         <color indexed="8"/>
       </top>
@@ -1031,11 +1044,115 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
       </left>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1043,7 +1160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1078,27 +1195,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1106,9 +1216,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1116,20 +1226,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1137,29 +1247,29 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="33" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1174,9 +1284,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1186,16 +1293,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1208,24 +1305,68 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1637,50 +1778,52 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="D29" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="7" width="23.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="23.5" style="1" customWidth="1"/>
+    <col min="7" max="9" width="20.1640625" style="28" customWidth="1"/>
+    <col min="10" max="10" width="23.5" style="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="28" style="1" customWidth="1"/>
-    <col min="15" max="15" width="33.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="1"/>
+    <col min="12" max="12" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="6.83203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="28" style="1" customWidth="1"/>
+    <col min="18" max="18" width="33.33203125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19">
+    <row r="1" spans="1:17" ht="19">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:17">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:17">
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-    </row>
-    <row r="5" spans="1:14">
+    <row r="4" spans="1:17">
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1689,13 +1832,15 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1706,14 +1851,16 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="39"/>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="34"/>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1721,17 +1868,19 @@
       <c r="C7" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="39"/>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="34"/>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1739,17 +1888,19 @@
       <c r="C8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="39"/>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="34"/>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" s="3" t="s">
         <v>71</v>
       </c>
@@ -1757,57 +1908,63 @@
       <c r="C9" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="H9" s="41"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="39"/>
-    </row>
-    <row r="10" spans="1:14" ht="45">
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="34"/>
+    </row>
+    <row r="10" spans="1:17" ht="45">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="74" t="s">
+      <c r="C10" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="39"/>
-    </row>
-    <row r="11" spans="1:14" ht="29" customHeight="1">
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="34"/>
+    </row>
+    <row r="11" spans="1:17" ht="29" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="82" t="s">
+      <c r="C11" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="83"/>
-      <c r="E11" s="83"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="72"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="61"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="61"/>
+      <c r="N11" s="61"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="33"/>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -1818,37 +1975,42 @@
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-    </row>
-    <row r="13" spans="1:14" s="33" customFormat="1">
-      <c r="A13" s="63" t="s">
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="33"/>
+    </row>
+    <row r="13" spans="1:17" s="28" customFormat="1">
+      <c r="A13" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="65"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="60"/>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="70"/>
-      <c r="L13"/>
-    </row>
-    <row r="14" spans="1:14" s="33" customFormat="1">
-      <c r="A14" s="63" t="s">
+      <c r="G13"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="65"/>
+      <c r="O13"/>
+    </row>
+    <row r="14" spans="1:17" s="28" customFormat="1">
+      <c r="A14" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="65" t="s">
+      <c r="B14" s="59"/>
+      <c r="C14" s="60" t="s">
         <v>45</v>
       </c>
       <c r="D14" t="s">
@@ -1856,156 +2018,182 @@
       </c>
       <c r="E14"/>
       <c r="F14"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="67"/>
-      <c r="J14" s="67"/>
-      <c r="K14" s="70"/>
-      <c r="L14"/>
-    </row>
-    <row r="15" spans="1:14" s="33" customFormat="1">
-      <c r="A15" s="63" t="s">
+      <c r="G14"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="65"/>
+      <c r="O14"/>
+    </row>
+    <row r="15" spans="1:17" s="28" customFormat="1">
+      <c r="A15" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="64"/>
-      <c r="C15" s="65"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="60"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="70"/>
-      <c r="L15"/>
-    </row>
-    <row r="16" spans="1:14" s="33" customFormat="1">
-      <c r="A16" s="63" t="s">
+      <c r="G15"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="86"/>
+      <c r="J15" s="62"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="62"/>
+      <c r="N15" s="65"/>
+      <c r="O15"/>
+    </row>
+    <row r="16" spans="1:17" s="28" customFormat="1">
+      <c r="A16" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="64"/>
-      <c r="C16" s="65" t="s">
+      <c r="B16" s="59"/>
+      <c r="C16" s="60" t="s">
         <v>45</v>
       </c>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="70"/>
-      <c r="L16"/>
-    </row>
-    <row r="17" spans="1:16" s="33" customFormat="1">
-      <c r="A17" s="63" t="s">
+      <c r="G16"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="62"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="62"/>
+      <c r="N16" s="65"/>
+      <c r="O16"/>
+    </row>
+    <row r="17" spans="1:19" s="28" customFormat="1">
+      <c r="A17" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="64"/>
-      <c r="C17" s="65" t="s">
+      <c r="B17" s="59"/>
+      <c r="C17" s="60" t="s">
         <v>45</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="70"/>
-      <c r="L17"/>
-    </row>
-    <row r="18" spans="1:16" s="33" customFormat="1">
-      <c r="A18" s="63" t="s">
+      <c r="G17"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="65"/>
+      <c r="O17"/>
+    </row>
+    <row r="18" spans="1:19" s="28" customFormat="1">
+      <c r="A18" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="64"/>
-      <c r="C18" s="65" t="s">
+      <c r="B18" s="59"/>
+      <c r="C18" s="60" t="s">
         <v>45</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="70"/>
-      <c r="L18"/>
-    </row>
-    <row r="19" spans="1:16" s="41" customFormat="1">
-      <c r="A19" s="38"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38"/>
-    </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="31" t="s">
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="62"/>
+      <c r="K18" s="62"/>
+      <c r="L18" s="62"/>
+      <c r="M18" s="62"/>
+      <c r="N18" s="65"/>
+      <c r="O18"/>
+    </row>
+    <row r="19" spans="1:19" s="36" customFormat="1">
+      <c r="A19" s="33"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="87"/>
+      <c r="I19" s="87"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="33"/>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33"/>
-    </row>
-    <row r="21" spans="1:16">
-      <c r="A21" s="34" t="s">
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="28"/>
+      <c r="S20" s="28"/>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="79"/>
-      <c r="H21" s="68"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="68"/>
-      <c r="K21" s="68"/>
-      <c r="L21" s="68"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="B21" s="30"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="90"/>
+      <c r="G21" s="80"/>
+      <c r="H21" s="87"/>
+      <c r="I21" s="87"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="63"/>
+      <c r="L21" s="63"/>
+      <c r="M21" s="63"/>
+      <c r="N21" s="63"/>
+      <c r="O21" s="63"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="28"/>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="10"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="39"/>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="91"/>
+      <c r="G22"/>
+      <c r="H22" s="86"/>
+      <c r="I22" s="86"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="34"/>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -2013,256 +2201,287 @@
       <c r="C23" s="7"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="80"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="39"/>
-    </row>
-    <row r="24" spans="1:16">
-      <c r="A24" s="38"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="39"/>
-    </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="31" t="s">
+      <c r="F23" s="92"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="34"/>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="A24" s="33"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="87"/>
+      <c r="I24" s="87"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="34"/>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="78"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="45"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="45"/>
-    </row>
-    <row r="26" spans="1:16">
-      <c r="A26" s="49" t="s">
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="81"/>
+      <c r="H25" s="88"/>
+      <c r="I25" s="88"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="41"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="40"/>
+      <c r="R25" s="40"/>
+      <c r="S25" s="40"/>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="79"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="68"/>
-      <c r="L26" s="68"/>
-      <c r="M26" s="46"/>
-      <c r="N26" s="47"/>
-      <c r="O26" s="47"/>
-      <c r="P26" s="39"/>
-    </row>
-    <row r="27" spans="1:16">
-      <c r="A27" s="52"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="81"/>
+      <c r="H26" s="88"/>
+      <c r="I26" s="88"/>
+      <c r="J26" s="63"/>
+      <c r="K26" s="63"/>
+      <c r="L26" s="63"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="63"/>
+      <c r="O26" s="63"/>
+      <c r="P26" s="41"/>
+      <c r="Q26" s="42"/>
+      <c r="R26" s="42"/>
+      <c r="S26" s="34"/>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="A27" s="47"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="94"/>
       <c r="G27" s="81"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="69"/>
-      <c r="J27" s="69"/>
-      <c r="K27" s="69"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="40"/>
-      <c r="O27" s="40"/>
-      <c r="P27" s="39"/>
-    </row>
-    <row r="28" spans="1:16">
-      <c r="A28" s="52"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="81"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="69"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="40"/>
-      <c r="N28" s="40"/>
-      <c r="O28" s="40"/>
-      <c r="P28" s="39"/>
-    </row>
-    <row r="29" spans="1:16">
-      <c r="A29" s="53"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="81"/>
-      <c r="H29" s="69"/>
-      <c r="I29" s="69"/>
-      <c r="J29" s="69"/>
-      <c r="K29" s="69"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="40"/>
-      <c r="N29" s="40"/>
-      <c r="O29" s="40"/>
-      <c r="P29" s="39"/>
-    </row>
-    <row r="30" spans="1:16" s="41" customFormat="1">
-      <c r="A30" s="38"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
-    </row>
-    <row r="31" spans="1:16">
-      <c r="A31" s="31" t="s">
+      <c r="H27" s="88"/>
+      <c r="I27" s="88"/>
+      <c r="J27" s="64"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="64"/>
+      <c r="N27" s="64"/>
+      <c r="O27" s="33"/>
+      <c r="P27" s="35"/>
+      <c r="Q27" s="35"/>
+      <c r="R27" s="35"/>
+      <c r="S27" s="34"/>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28" s="47"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="95"/>
+      <c r="G28"/>
+      <c r="H28" s="86"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="64"/>
+      <c r="K28" s="64"/>
+      <c r="L28" s="64"/>
+      <c r="M28" s="64"/>
+      <c r="N28" s="64"/>
+      <c r="O28" s="33"/>
+      <c r="P28" s="35"/>
+      <c r="Q28" s="35"/>
+      <c r="R28" s="35"/>
+      <c r="S28" s="34"/>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29" s="48"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="96"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="64"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="64"/>
+      <c r="O29" s="33"/>
+      <c r="P29" s="35"/>
+      <c r="Q29" s="35"/>
+      <c r="R29" s="35"/>
+      <c r="S29" s="34"/>
+    </row>
+    <row r="30" spans="1:19" s="36" customFormat="1">
+      <c r="A30" s="33"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="33"/>
+      <c r="O30" s="33"/>
+      <c r="P30" s="33"/>
+      <c r="Q30" s="33"/>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="45"/>
-      <c r="P31" s="45"/>
-    </row>
-    <row r="32" spans="1:16">
-      <c r="A32" s="49" t="s">
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="89"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="41"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="40"/>
+      <c r="Q31" s="40"/>
+      <c r="R31" s="40"/>
+      <c r="S31" s="40"/>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="79"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="68"/>
-      <c r="K32" s="68"/>
-      <c r="L32" s="68"/>
-      <c r="M32" s="46"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="47"/>
-      <c r="P32" s="39"/>
-    </row>
-    <row r="33" spans="1:16">
-      <c r="A33" s="52">
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="93"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="63"/>
+      <c r="O32" s="63"/>
+      <c r="P32" s="41"/>
+      <c r="Q32" s="42"/>
+      <c r="R32" s="42"/>
+      <c r="S32" s="34"/>
+    </row>
+    <row r="33" spans="1:19">
+      <c r="A33" s="47">
         <v>1</v>
       </c>
-      <c r="B33" s="48" t="s">
+      <c r="B33" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="81"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="69"/>
-      <c r="J33" s="69"/>
-      <c r="K33" s="69"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="40"/>
-      <c r="N33" s="40"/>
-      <c r="O33" s="40"/>
-      <c r="P33" s="39"/>
-    </row>
-    <row r="34" spans="1:16">
-      <c r="A34" s="52"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="81"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69"/>
-      <c r="L34" s="38"/>
-      <c r="M34" s="40"/>
-      <c r="N34" s="40"/>
-      <c r="O34" s="40"/>
-      <c r="P34" s="39"/>
-    </row>
-    <row r="35" spans="1:16">
-      <c r="A35" s="53"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="81"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="69"/>
-      <c r="J35" s="69"/>
-      <c r="K35" s="69"/>
-      <c r="L35" s="38"/>
-      <c r="M35" s="40"/>
-      <c r="N35" s="40"/>
-      <c r="O35" s="40"/>
-      <c r="P35" s="39"/>
-    </row>
-    <row r="36" spans="1:16">
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="94"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="64"/>
+      <c r="K33" s="64"/>
+      <c r="L33" s="64"/>
+      <c r="M33" s="64"/>
+      <c r="N33" s="64"/>
+      <c r="O33" s="33"/>
+      <c r="P33" s="35"/>
+      <c r="Q33" s="35"/>
+      <c r="R33" s="35"/>
+      <c r="S33" s="34"/>
+    </row>
+    <row r="34" spans="1:19">
+      <c r="A34" s="47"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="95"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="64"/>
+      <c r="K34" s="64"/>
+      <c r="L34" s="64"/>
+      <c r="M34" s="64"/>
+      <c r="N34" s="64"/>
+      <c r="O34" s="33"/>
+      <c r="P34" s="35"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="35"/>
+      <c r="S34" s="34"/>
+    </row>
+    <row r="35" spans="1:19">
+      <c r="A35" s="48"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="96"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="64"/>
+      <c r="K35" s="64"/>
+      <c r="L35" s="64"/>
+      <c r="M35" s="64"/>
+      <c r="N35" s="64"/>
+      <c r="O35" s="33"/>
+      <c r="P35" s="35"/>
+      <c r="Q35" s="35"/>
+      <c r="R35" s="35"/>
+      <c r="S35" s="34"/>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
       <c r="M36" s="13"/>
-    </row>
-    <row r="37" spans="1:16">
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37" s="3" t="s">
         <v>11</v>
       </c>
@@ -2271,78 +2490,93 @@
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="59"/>
+      <c r="I37" s="59"/>
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
       <c r="L37" s="14"/>
       <c r="M37" s="14"/>
       <c r="N37" s="14"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="15"/>
-    </row>
-    <row r="38" spans="1:16" ht="13.5" customHeight="1">
-      <c r="A38" s="86" t="s">
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="15"/>
+    </row>
+    <row r="38" spans="1:19" ht="13.5" customHeight="1">
+      <c r="A38" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="86" t="s">
+      <c r="B38" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="85" t="s">
+      <c r="C38" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="85" t="s">
+      <c r="D38" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="87" t="s">
+      <c r="E38" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="F38" s="85" t="s">
+      <c r="F38" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="85" t="s">
+      <c r="G38" s="82" t="s">
+        <v>82</v>
+      </c>
+      <c r="H38" s="82" t="s">
+        <v>83</v>
+      </c>
+      <c r="I38" s="82" t="s">
+        <v>84</v>
+      </c>
+      <c r="J38" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="H38" s="87" t="s">
+      <c r="K38" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="I38" s="87" t="s">
+      <c r="L38" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="J38" s="90" t="s">
+      <c r="M38" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="K38" s="90" t="s">
+      <c r="N38" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="L38" s="85" t="s">
+      <c r="O38" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="M38" s="85"/>
-      <c r="N38" s="16"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="9"/>
-    </row>
-    <row r="39" spans="1:16">
-      <c r="A39" s="86"/>
-      <c r="B39" s="86"/>
-      <c r="C39" s="85"/>
-      <c r="D39" s="85"/>
-      <c r="E39" s="88"/>
-      <c r="F39" s="85"/>
-      <c r="G39" s="85"/>
-      <c r="H39" s="89"/>
-      <c r="I39" s="89"/>
-      <c r="J39" s="91"/>
-      <c r="K39" s="91"/>
-      <c r="L39" s="85"/>
-      <c r="M39" s="85"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="30"/>
-      <c r="P39" s="15"/>
-    </row>
-    <row r="40" spans="1:16">
+      <c r="P38" s="73"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="17"/>
+      <c r="S38" s="9"/>
+    </row>
+    <row r="39" spans="1:19">
+      <c r="A39" s="74"/>
+      <c r="B39" s="74"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="82"/>
+      <c r="H39" s="82"/>
+      <c r="I39" s="82"/>
+      <c r="J39" s="73"/>
+      <c r="K39" s="77"/>
+      <c r="L39" s="77"/>
+      <c r="M39" s="79"/>
+      <c r="N39" s="79"/>
+      <c r="O39" s="73"/>
+      <c r="P39" s="73"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="25"/>
+      <c r="S39" s="15"/>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" s="19">
         <v>1</v>
       </c>
@@ -2359,26 +2593,29 @@
       <c r="F40" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G40" s="21" t="s">
+      <c r="G40" s="83"/>
+      <c r="H40" s="83"/>
+      <c r="I40" s="83"/>
+      <c r="J40" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="H40" s="21"/>
-      <c r="I40" s="71"/>
-      <c r="J40" s="71" t="s">
+      <c r="K40" s="21"/>
+      <c r="L40" s="66"/>
+      <c r="M40" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="K40" s="71" t="s">
+      <c r="N40" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="L40" s="21" t="s">
+      <c r="O40" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="15"/>
-    </row>
-    <row r="41" spans="1:16" ht="60">
+      <c r="P40" s="22"/>
+      <c r="Q40" s="22"/>
+      <c r="R40" s="24"/>
+      <c r="S40" s="15"/>
+    </row>
+    <row r="41" spans="1:19" ht="60">
       <c r="A41" s="19">
         <f>A40+1</f>
         <v>2</v>
@@ -2390,26 +2627,29 @@
         <v>53</v>
       </c>
       <c r="D41" s="21"/>
-      <c r="E41" s="75" t="s">
+      <c r="E41" s="69" t="s">
         <v>68</v>
       </c>
       <c r="F41" s="21"/>
-      <c r="G41" s="21">
+      <c r="G41" s="84"/>
+      <c r="H41" s="84"/>
+      <c r="I41" s="84"/>
+      <c r="J41" s="21">
         <v>0</v>
       </c>
-      <c r="H41" s="21"/>
-      <c r="I41" s="71"/>
-      <c r="J41" s="71"/>
-      <c r="K41" s="71" t="s">
+      <c r="K41" s="21"/>
+      <c r="L41" s="66"/>
+      <c r="M41" s="66"/>
+      <c r="N41" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="L41" s="21"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="22"/>
-      <c r="O41" s="29"/>
-      <c r="P41" s="15"/>
-    </row>
-    <row r="42" spans="1:16">
+      <c r="O41" s="21"/>
+      <c r="P41" s="22"/>
+      <c r="Q41" s="22"/>
+      <c r="R41" s="24"/>
+      <c r="S41" s="15"/>
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42" s="19">
         <f t="shared" ref="A42:A44" si="0">A41+1</f>
         <v>3</v>
@@ -2427,24 +2667,27 @@
       <c r="F42" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="G42" s="21" t="s">
+      <c r="G42" s="84"/>
+      <c r="H42" s="84"/>
+      <c r="I42" s="84"/>
+      <c r="J42" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="H42" s="21"/>
-      <c r="I42" s="71" t="s">
+      <c r="K42" s="21"/>
+      <c r="L42" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="J42" s="71"/>
-      <c r="K42" s="71"/>
-      <c r="L42" s="21" t="s">
+      <c r="M42" s="66"/>
+      <c r="N42" s="66"/>
+      <c r="O42" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="M42" s="22"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="23"/>
-      <c r="P42" s="15"/>
-    </row>
-    <row r="43" spans="1:16" ht="30">
+      <c r="P42" s="22"/>
+      <c r="Q42" s="22"/>
+      <c r="R42" s="23"/>
+      <c r="S42" s="15"/>
+    </row>
+    <row r="43" spans="1:19" ht="30">
       <c r="A43" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2456,26 +2699,29 @@
         <v>25</v>
       </c>
       <c r="D43" s="21"/>
-      <c r="E43" s="75" t="s">
+      <c r="E43" s="69" t="s">
         <v>66</v>
       </c>
       <c r="F43" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="71"/>
-      <c r="J43" s="71"/>
-      <c r="K43" s="71"/>
-      <c r="L43" s="21" t="s">
+      <c r="G43" s="84"/>
+      <c r="H43" s="84"/>
+      <c r="I43" s="84"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="66"/>
+      <c r="M43" s="66"/>
+      <c r="N43" s="66"/>
+      <c r="O43" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
-      <c r="O43" s="23"/>
-      <c r="P43" s="15"/>
-    </row>
-    <row r="44" spans="1:16" ht="15">
+      <c r="P43" s="22"/>
+      <c r="Q43" s="22"/>
+      <c r="R43" s="23"/>
+      <c r="S43" s="15"/>
+    </row>
+    <row r="44" spans="1:19" ht="15">
       <c r="A44" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2487,90 +2733,146 @@
         <v>20</v>
       </c>
       <c r="D44" s="21"/>
-      <c r="E44" s="73" t="s">
+      <c r="E44" s="67" t="s">
         <v>69</v>
       </c>
       <c r="F44" s="21"/>
-      <c r="G44" s="21" t="s">
+      <c r="G44" s="85"/>
+      <c r="H44" s="85"/>
+      <c r="I44" s="85"/>
+      <c r="J44" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="H44" s="21"/>
-      <c r="I44" s="71"/>
-      <c r="J44" s="71"/>
-      <c r="K44" s="71"/>
-      <c r="L44" s="21" t="s">
+      <c r="K44" s="21"/>
+      <c r="L44" s="66"/>
+      <c r="M44" s="66"/>
+      <c r="N44" s="66"/>
+      <c r="O44" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="23"/>
-      <c r="P44" s="15"/>
-    </row>
-    <row r="45" spans="1:16">
-      <c r="A45" s="24">
+      <c r="P44" s="22"/>
+      <c r="Q44" s="22"/>
+      <c r="R44" s="23"/>
+      <c r="S44" s="15"/>
+    </row>
+    <row r="45" spans="1:19">
+      <c r="A45" s="103">
         <v>6</v>
       </c>
-      <c r="B45" s="25" t="s">
+      <c r="B45" s="104" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="26" t="s">
+      <c r="C45" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="72" t="s">
+      <c r="H45" s="84"/>
+      <c r="I45" s="85" t="s">
+        <v>86</v>
+      </c>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="J45" s="72"/>
-      <c r="K45" s="72"/>
-      <c r="L45" s="26" t="s">
+      <c r="M45" s="66"/>
+      <c r="N45" s="66"/>
+      <c r="O45" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="M45" s="27"/>
-      <c r="N45" s="27"/>
-      <c r="O45" s="28"/>
-      <c r="P45" s="15"/>
-    </row>
-    <row r="46" spans="1:16">
-      <c r="A46" s="24"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="72"/>
-      <c r="J46" s="72"/>
-      <c r="K46" s="72"/>
-      <c r="L46" s="26"/>
-      <c r="M46" s="27"/>
-      <c r="N46" s="27"/>
-      <c r="O46" s="28"/>
-      <c r="P46" s="15"/>
+      <c r="P45" s="22"/>
+      <c r="Q45" s="22"/>
+      <c r="R45" s="23"/>
+      <c r="S45" s="15"/>
+    </row>
+    <row r="46" spans="1:19">
+      <c r="A46" s="97"/>
+      <c r="B46" s="98"/>
+      <c r="C46" s="99"/>
+      <c r="D46" s="99"/>
+      <c r="E46" s="99"/>
+      <c r="F46" s="99"/>
+      <c r="G46" s="106"/>
+      <c r="H46" s="107"/>
+      <c r="I46" s="107"/>
+      <c r="J46" s="99"/>
+      <c r="K46" s="99"/>
+      <c r="L46" s="100"/>
+      <c r="M46" s="100"/>
+      <c r="N46" s="100"/>
+      <c r="O46" s="99"/>
+      <c r="P46" s="101"/>
+      <c r="Q46" s="101"/>
+      <c r="R46" s="102"/>
+      <c r="S46" s="15"/>
+    </row>
+    <row r="47" spans="1:19">
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
+    </row>
+    <row r="48" spans="1:19">
+      <c r="G48" s="105"/>
+      <c r="H48" s="105"/>
+      <c r="I48" s="105"/>
+    </row>
+    <row r="49" spans="7:9">
+      <c r="G49" s="41"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="41"/>
+    </row>
+    <row r="50" spans="7:9">
+      <c r="G50" s="41"/>
+      <c r="H50" s="41"/>
+      <c r="I50" s="41"/>
+    </row>
+    <row r="51" spans="7:9">
+      <c r="G51" s="41"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="41"/>
+    </row>
+    <row r="52" spans="7:9">
+      <c r="G52" s="41"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="41"/>
+    </row>
+    <row r="53" spans="7:9">
+      <c r="G53" s="41"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="41"/>
+    </row>
+    <row r="54" spans="7:9">
+      <c r="G54" s="41"/>
+      <c r="H54" s="41"/>
+      <c r="I54" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="16">
     <mergeCell ref="C11:F11"/>
-    <mergeCell ref="L38:M39"/>
+    <mergeCell ref="O38:P39"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="F38:F39"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="E38:E39"/>
-    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="M38:M39"/>
     <mergeCell ref="K38:K39"/>
     <mergeCell ref="J38:J39"/>
+    <mergeCell ref="G38:G39"/>
     <mergeCell ref="H38:H39"/>
-    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="I38:I39"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F62:K62" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F62 J62:N62" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2583,7 +2885,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15 H40:H46" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15 K40:K46" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>isAbstract</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{061A2328-C320-074B-A7A0-1D5ADA23E625}">
@@ -2605,7 +2907,7 @@
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>
           </x14:formula1>
-          <xm:sqref>I40:K46</xm:sqref>
+          <xm:sqref>L40:N46</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2621,112 +2923,112 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="56" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="56" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="56" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" style="56" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="56" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" style="56" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="56" customWidth="1"/>
-    <col min="10" max="10" width="18.5" style="56" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="56" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="56" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="56" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" style="56" bestFit="1" customWidth="1"/>
-    <col min="15" max="260" width="8.83203125" style="56" customWidth="1"/>
-    <col min="261" max="16384" width="10.83203125" style="56"/>
+    <col min="1" max="3" width="8.83203125" style="51" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="51" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="51" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="51" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" style="51" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="51" customWidth="1"/>
+    <col min="10" max="10" width="18.5" style="51" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="51" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="51" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="15" max="260" width="8.83203125" style="51" customWidth="1"/>
+    <col min="261" max="16384" width="10.83203125" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="55" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="55"/>
+      <c r="Q1" s="50"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="57" t="s">
+      <c r="H3" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="57" t="s">
+      <c r="J3" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="57" t="s">
+      <c r="L3" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="57" t="s">
+      <c r="N3" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="57" t="s">
+      <c r="P3" s="52" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="B4" s="58"/>
-      <c r="D4" s="61" t="s">
+      <c r="B4" s="53"/>
+      <c r="D4" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="H4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="N4" s="59"/>
-      <c r="P4" s="59"/>
+      <c r="H4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="P4" s="54"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="H5" s="61" t="s">
+      <c r="D5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="H5" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="61" t="s">
+      <c r="J5" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="61" t="s">
+      <c r="L5" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="61" t="s">
+      <c r="N5" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="P5" s="61" t="s">
+      <c r="P5" s="56" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="B6" s="62"/>
+      <c r="B6" s="57"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>

</xml_diff>

<commit_message>
0.0.10: If field type for kotlin defined, force select kotlin preferred generic and defaults.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B7331E-8C49-7C44-AD1C-52C242E7CC10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E30F37-BC71-A547-A94D-EBD5E91545B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="5380" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="88">
   <si>
     <t>クラス名</t>
   </si>
@@ -495,6 +495,10 @@
   </si>
   <si>
     <t>@JsonProperty</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>new ApiTelegram()</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1780,8 +1784,8 @@
   </sheetPr>
   <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D29" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2767,7 +2771,9 @@
       </c>
       <c r="D45" s="21"/>
       <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
+      <c r="F45" s="21" t="s">
+        <v>87</v>
+      </c>
       <c r="G45" s="84" t="s">
         <v>74</v>
       </c>
@@ -2781,7 +2787,9 @@
         <v>45</v>
       </c>
       <c r="M45" s="66"/>
-      <c r="N45" s="66"/>
+      <c r="N45" s="66" t="s">
+        <v>45</v>
+      </c>
       <c r="O45" s="21" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
0.0.11: Adapt to delegate.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E30F37-BC71-A547-A94D-EBD5E91545B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D60BDF-5A60-2B43-B765-F1A9FC02D31A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="5380" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="2220" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="94">
   <si>
     <t>クラス名</t>
   </si>
@@ -124,9 +124,6 @@
   <si>
     <t>array</t>
     <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>バリューオブジェクト定義(php)・継承</t>
   </si>
   <si>
     <t>arrayObject</t>
@@ -494,11 +491,51 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>@JsonProperty</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>new ApiTelegram()</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>バリューオブジェクト定義(Kt)・委譲</t>
+    <rPh sb="17" eb="19">
+      <t xml:space="preserve">イジョウ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>総称型</t>
+    <rPh sb="0" eb="2">
+      <t>ソウショウガタ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>説明</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">セツメイ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>blanco.restgerator.valueobject.ApiTelegram</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>委譲のテストです</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">イジョウ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>バリューオブジェクト定義(php)・継承</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>@JsonProperty
+@hoge</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -596,7 +633,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -1159,12 +1196,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1297,43 +1375,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1371,6 +1416,53 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1782,10 +1874,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S54"/>
+  <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" topLeftCell="C34" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1810,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1850,7 +1942,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -1870,7 +1962,7 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="32"/>
@@ -1886,11 +1978,11 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="32"/>
@@ -1906,17 +1998,17 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="32"/>
       <c r="F9" s="11"/>
       <c r="G9" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H9" s="40"/>
       <c r="I9" s="40"/>
@@ -1928,11 +2020,11 @@
     </row>
     <row r="10" spans="1:17" ht="45">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32"/>
@@ -1951,12 +2043,12 @@
         <v>2</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="70" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="72"/>
+      <c r="C11" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="98"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="99"/>
       <c r="H11" s="40"/>
       <c r="I11" s="40"/>
       <c r="J11" s="61"/>
@@ -1992,7 +2084,7 @@
     </row>
     <row r="13" spans="1:17" s="28" customFormat="1">
       <c r="A13" s="58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="59"/>
       <c r="C13" s="60"/>
@@ -2000,8 +2092,8 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
       <c r="J13" s="62"/>
       <c r="K13" s="62"/>
       <c r="L13" s="62"/>
@@ -2011,20 +2103,20 @@
     </row>
     <row r="14" spans="1:17" s="28" customFormat="1">
       <c r="A14" s="58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="59"/>
       <c r="C14" s="60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="75"/>
       <c r="J14" s="62"/>
       <c r="K14" s="62"/>
       <c r="L14" s="62"/>
@@ -2034,7 +2126,7 @@
     </row>
     <row r="15" spans="1:17" s="28" customFormat="1">
       <c r="A15" s="58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="59"/>
       <c r="C15" s="60"/>
@@ -2042,8 +2134,8 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="86"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="75"/>
       <c r="J15" s="62"/>
       <c r="K15" s="62"/>
       <c r="L15" s="62"/>
@@ -2053,18 +2145,18 @@
     </row>
     <row r="16" spans="1:17" s="28" customFormat="1">
       <c r="A16" s="58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="59"/>
       <c r="C16" s="60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
-      <c r="H16" s="86"/>
-      <c r="I16" s="86"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="75"/>
       <c r="J16" s="62"/>
       <c r="K16" s="62"/>
       <c r="L16" s="62"/>
@@ -2074,18 +2166,16 @@
     </row>
     <row r="17" spans="1:19" s="28" customFormat="1">
       <c r="A17" s="58" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="59"/>
-      <c r="C17" s="60" t="s">
-        <v>45</v>
-      </c>
+      <c r="C17" s="60"/>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="86"/>
+      <c r="H17" s="75"/>
+      <c r="I17" s="75"/>
       <c r="J17" s="62"/>
       <c r="K17" s="62"/>
       <c r="L17" s="62"/>
@@ -2095,11 +2185,11 @@
     </row>
     <row r="18" spans="1:19" s="28" customFormat="1">
       <c r="A18" s="58" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="59"/>
       <c r="C18" s="60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
@@ -2120,9 +2210,9 @@
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
       <c r="F19" s="33"/>
-      <c r="G19" s="80"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="87"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="76"/>
       <c r="J19" s="33"/>
       <c r="K19" s="33"/>
       <c r="L19" s="33"/>
@@ -2134,16 +2224,16 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="26" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
       <c r="D20" s="27"/>
       <c r="E20" s="27"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="80"/>
-      <c r="H20" s="87"/>
-      <c r="I20" s="87"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="76"/>
       <c r="J20" s="41"/>
       <c r="K20" s="41"/>
       <c r="L20" s="41"/>
@@ -2163,10 +2253,10 @@
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
       <c r="E21" s="31"/>
-      <c r="F21" s="90"/>
-      <c r="G21" s="80"/>
-      <c r="H21" s="87"/>
-      <c r="I21" s="87"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="76"/>
       <c r="J21" s="63"/>
       <c r="K21" s="63"/>
       <c r="L21" s="63"/>
@@ -2180,16 +2270,16 @@
     </row>
     <row r="22" spans="1:19">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="10"/>
       <c r="D22" s="32"/>
       <c r="E22" s="32"/>
-      <c r="F22" s="91"/>
+      <c r="F22" s="80"/>
       <c r="G22"/>
-      <c r="H22" s="86"/>
-      <c r="I22" s="86"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="75"/>
       <c r="J22" s="33"/>
       <c r="K22" s="33"/>
       <c r="L22" s="33"/>
@@ -2199,13 +2289,13 @@
     </row>
     <row r="23" spans="1:19">
       <c r="A23" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
-      <c r="F23" s="92"/>
+      <c r="F23" s="81"/>
       <c r="H23" s="40"/>
       <c r="I23" s="40"/>
       <c r="J23" s="33"/>
@@ -2222,9 +2312,9 @@
       <c r="D24" s="33"/>
       <c r="E24" s="33"/>
       <c r="F24" s="33"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="76"/>
       <c r="J24" s="33"/>
       <c r="K24" s="33"/>
       <c r="L24" s="33"/>
@@ -2234,16 +2324,16 @@
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
-      <c r="F25" s="89"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="88"/>
-      <c r="I25" s="88"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="77"/>
+      <c r="I25" s="77"/>
       <c r="J25" s="41"/>
       <c r="K25" s="41"/>
       <c r="L25" s="41"/>
@@ -2257,18 +2347,18 @@
     </row>
     <row r="26" spans="1:19">
       <c r="A26" s="44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="39"/>
       <c r="D26" s="39"/>
       <c r="E26" s="39"/>
-      <c r="F26" s="93"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="88"/>
-      <c r="I26" s="88"/>
+      <c r="F26" s="82"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="77"/>
+      <c r="I26" s="77"/>
       <c r="J26" s="63"/>
       <c r="K26" s="63"/>
       <c r="L26" s="63"/>
@@ -2286,10 +2376,10 @@
       <c r="C27" s="37"/>
       <c r="D27" s="37"/>
       <c r="E27" s="37"/>
-      <c r="F27" s="94"/>
-      <c r="G27" s="81"/>
-      <c r="H27" s="88"/>
-      <c r="I27" s="88"/>
+      <c r="F27" s="83"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="77"/>
+      <c r="I27" s="77"/>
       <c r="J27" s="64"/>
       <c r="K27" s="64"/>
       <c r="L27" s="64"/>
@@ -2307,10 +2397,10 @@
       <c r="C28" s="38"/>
       <c r="D28" s="38"/>
       <c r="E28" s="38"/>
-      <c r="F28" s="95"/>
+      <c r="F28" s="84"/>
       <c r="G28"/>
-      <c r="H28" s="86"/>
-      <c r="I28" s="86"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="75"/>
       <c r="J28" s="64"/>
       <c r="K28" s="64"/>
       <c r="L28" s="64"/>
@@ -2328,7 +2418,7 @@
       <c r="C29" s="46"/>
       <c r="D29" s="46"/>
       <c r="E29" s="46"/>
-      <c r="F29" s="96"/>
+      <c r="F29" s="85"/>
       <c r="H29" s="40"/>
       <c r="I29" s="40"/>
       <c r="J29" s="64"/>
@@ -2360,527 +2450,690 @@
       <c r="P30" s="33"/>
       <c r="Q30" s="33"/>
     </row>
-    <row r="31" spans="1:19">
-      <c r="A31" s="26" t="s">
+    <row r="31" spans="1:19" s="28" customFormat="1">
+      <c r="A31" s="108" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="59"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="109"/>
+    </row>
+    <row r="32" spans="1:19" s="28" customFormat="1">
+      <c r="A32" s="101" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="101" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="107" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="107" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" s="107" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32" s="113"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="70"/>
+      <c r="J32" s="70"/>
+      <c r="K32" s="70"/>
+    </row>
+    <row r="33" spans="1:19" s="28" customFormat="1">
+      <c r="A33" s="101"/>
+      <c r="B33" s="101"/>
+      <c r="C33" s="107"/>
+      <c r="D33" s="107"/>
+      <c r="E33" s="107"/>
+      <c r="F33" s="113"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="70"/>
+      <c r="K33" s="70"/>
+    </row>
+    <row r="34" spans="1:19" s="28" customFormat="1">
+      <c r="A34" s="19">
+        <v>1</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="73" t="s">
+        <v>90</v>
+      </c>
+      <c r="D34" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="73" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" s="114"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="70"/>
+      <c r="J34" s="70"/>
+      <c r="K34" s="70"/>
+      <c r="L34" s="70"/>
+    </row>
+    <row r="35" spans="1:19" s="28" customFormat="1">
+      <c r="A35" s="19"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="73"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="114"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="70"/>
+      <c r="J35" s="70"/>
+      <c r="K35" s="70"/>
+      <c r="L35" s="70"/>
+    </row>
+    <row r="36" spans="1:19" s="28" customFormat="1">
+      <c r="A36" s="19"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="73"/>
+      <c r="D36" s="73"/>
+      <c r="E36" s="73"/>
+      <c r="F36" s="114"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="70"/>
+      <c r="J36" s="70"/>
+      <c r="K36" s="70"/>
+      <c r="L36" s="70"/>
+    </row>
+    <row r="37" spans="1:19" s="28" customFormat="1">
+      <c r="A37" s="19"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="73"/>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="114"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="70"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="70"/>
+      <c r="L37" s="70"/>
+    </row>
+    <row r="38" spans="1:19" s="28" customFormat="1">
+      <c r="A38" s="19"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="73"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="114"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="70"/>
+      <c r="I38" s="70"/>
+      <c r="J38" s="70"/>
+      <c r="K38" s="70"/>
+      <c r="L38" s="70"/>
+    </row>
+    <row r="39" spans="1:19" s="28" customFormat="1">
+      <c r="A39" s="110"/>
+      <c r="B39" s="111"/>
+      <c r="C39" s="112"/>
+      <c r="D39" s="112"/>
+      <c r="E39" s="112"/>
+      <c r="F39" s="115"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="70"/>
+      <c r="J39" s="70"/>
+      <c r="K39" s="70"/>
+      <c r="L39" s="70"/>
+    </row>
+    <row r="40" spans="1:19" s="28" customFormat="1">
+      <c r="A40"/>
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40" s="71"/>
+      <c r="M40"/>
+    </row>
+    <row r="41" spans="1:19">
+      <c r="A41" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="78"/>
+      <c r="H41" s="40"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="41"/>
+      <c r="K41" s="41"/>
+      <c r="L41" s="41"/>
+      <c r="M41" s="41"/>
+      <c r="N41" s="41"/>
+      <c r="O41" s="41"/>
+      <c r="P41" s="40"/>
+      <c r="Q41" s="40"/>
+      <c r="R41" s="40"/>
+      <c r="S41" s="40"/>
+    </row>
+    <row r="42" spans="1:19">
+      <c r="A42" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="89"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="41"/>
-      <c r="M31" s="41"/>
-      <c r="N31" s="41"/>
-      <c r="O31" s="41"/>
-      <c r="P31" s="40"/>
-      <c r="Q31" s="40"/>
-      <c r="R31" s="40"/>
-      <c r="S31" s="40"/>
-    </row>
-    <row r="32" spans="1:19">
-      <c r="A32" s="44" t="s">
+      <c r="B42" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="82"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="40"/>
+      <c r="J42" s="63"/>
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63"/>
+      <c r="O42" s="63"/>
+      <c r="P42" s="41"/>
+      <c r="Q42" s="42"/>
+      <c r="R42" s="42"/>
+      <c r="S42" s="34"/>
+    </row>
+    <row r="43" spans="1:19">
+      <c r="A43" s="47">
+        <v>1</v>
+      </c>
+      <c r="B43" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="83"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="64"/>
+      <c r="K43" s="64"/>
+      <c r="L43" s="64"/>
+      <c r="M43" s="64"/>
+      <c r="N43" s="64"/>
+      <c r="O43" s="33"/>
+      <c r="P43" s="35"/>
+      <c r="Q43" s="35"/>
+      <c r="R43" s="35"/>
+      <c r="S43" s="34"/>
+    </row>
+    <row r="44" spans="1:19">
+      <c r="A44" s="47"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="84"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="64"/>
+      <c r="K44" s="64"/>
+      <c r="L44" s="64"/>
+      <c r="M44" s="64"/>
+      <c r="N44" s="64"/>
+      <c r="O44" s="33"/>
+      <c r="P44" s="35"/>
+      <c r="Q44" s="35"/>
+      <c r="R44" s="35"/>
+      <c r="S44" s="34"/>
+    </row>
+    <row r="45" spans="1:19">
+      <c r="A45" s="48"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="85"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="64"/>
+      <c r="K45" s="64"/>
+      <c r="L45" s="64"/>
+      <c r="M45" s="64"/>
+      <c r="N45" s="64"/>
+      <c r="O45" s="33"/>
+      <c r="P45" s="35"/>
+      <c r="Q45" s="35"/>
+      <c r="R45" s="35"/>
+      <c r="S45" s="34"/>
+    </row>
+    <row r="46" spans="1:19">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="13"/>
+    </row>
+    <row r="47" spans="1:19">
+      <c r="A47" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="59"/>
+      <c r="H47" s="59"/>
+      <c r="I47" s="59"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="6"/>
+      <c r="S47" s="15"/>
+    </row>
+    <row r="48" spans="1:19" ht="13.5" customHeight="1">
+      <c r="A48" s="101" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="101" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="100" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="100" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="102" t="s">
+        <v>22</v>
+      </c>
+      <c r="F48" s="100" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="107" t="s">
+        <v>81</v>
+      </c>
+      <c r="H48" s="107" t="s">
+        <v>82</v>
+      </c>
+      <c r="I48" s="107" t="s">
+        <v>83</v>
+      </c>
+      <c r="J48" s="100" t="s">
+        <v>75</v>
+      </c>
+      <c r="K48" s="102" t="s">
+        <v>64</v>
+      </c>
+      <c r="L48" s="102" t="s">
+        <v>48</v>
+      </c>
+      <c r="M48" s="105" t="s">
+        <v>57</v>
+      </c>
+      <c r="N48" s="105" t="s">
+        <v>56</v>
+      </c>
+      <c r="O48" s="100" t="s">
+        <v>2</v>
+      </c>
+      <c r="P48" s="100"/>
+      <c r="Q48" s="16"/>
+      <c r="R48" s="17"/>
+      <c r="S48" s="9"/>
+    </row>
+    <row r="49" spans="1:19">
+      <c r="A49" s="101"/>
+      <c r="B49" s="101"/>
+      <c r="C49" s="100"/>
+      <c r="D49" s="100"/>
+      <c r="E49" s="103"/>
+      <c r="F49" s="100"/>
+      <c r="G49" s="107"/>
+      <c r="H49" s="107"/>
+      <c r="I49" s="107"/>
+      <c r="J49" s="100"/>
+      <c r="K49" s="104"/>
+      <c r="L49" s="104"/>
+      <c r="M49" s="106"/>
+      <c r="N49" s="106"/>
+      <c r="O49" s="100"/>
+      <c r="P49" s="100"/>
+      <c r="Q49" s="18"/>
+      <c r="R49" s="25"/>
+      <c r="S49" s="15"/>
+    </row>
+    <row r="50" spans="1:19">
+      <c r="A50" s="19">
+        <v>1</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F50" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="93"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="63"/>
-      <c r="K32" s="63"/>
-      <c r="L32" s="63"/>
-      <c r="M32" s="63"/>
-      <c r="N32" s="63"/>
-      <c r="O32" s="63"/>
-      <c r="P32" s="41"/>
-      <c r="Q32" s="42"/>
-      <c r="R32" s="42"/>
-      <c r="S32" s="34"/>
-    </row>
-    <row r="33" spans="1:19">
-      <c r="A33" s="47">
-        <v>1</v>
-      </c>
-      <c r="B33" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="94"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="64"/>
-      <c r="K33" s="64"/>
-      <c r="L33" s="64"/>
-      <c r="M33" s="64"/>
-      <c r="N33" s="64"/>
-      <c r="O33" s="33"/>
-      <c r="P33" s="35"/>
-      <c r="Q33" s="35"/>
-      <c r="R33" s="35"/>
-      <c r="S33" s="34"/>
-    </row>
-    <row r="34" spans="1:19">
-      <c r="A34" s="47"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="95"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="64"/>
-      <c r="K34" s="64"/>
-      <c r="L34" s="64"/>
-      <c r="M34" s="64"/>
-      <c r="N34" s="64"/>
-      <c r="O34" s="33"/>
-      <c r="P34" s="35"/>
-      <c r="Q34" s="35"/>
-      <c r="R34" s="35"/>
-      <c r="S34" s="34"/>
-    </row>
-    <row r="35" spans="1:19">
-      <c r="A35" s="48"/>
-      <c r="B35" s="45"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="96"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="40"/>
-      <c r="J35" s="64"/>
-      <c r="K35" s="64"/>
-      <c r="L35" s="64"/>
-      <c r="M35" s="64"/>
-      <c r="N35" s="64"/>
-      <c r="O35" s="33"/>
-      <c r="P35" s="35"/>
-      <c r="Q35" s="35"/>
-      <c r="R35" s="35"/>
-      <c r="S35" s="34"/>
-    </row>
-    <row r="36" spans="1:19">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-    </row>
-    <row r="37" spans="1:19">
-      <c r="A37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="59"/>
-      <c r="H37" s="59"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="6"/>
-      <c r="S37" s="15"/>
-    </row>
-    <row r="38" spans="1:19" ht="13.5" customHeight="1">
-      <c r="A38" s="74" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" s="74" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="73" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="73" t="s">
+      <c r="G50" s="72"/>
+      <c r="H50" s="72"/>
+      <c r="I50" s="72"/>
+      <c r="J50" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="K50" s="21"/>
+      <c r="L50" s="66"/>
+      <c r="M50" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="N50" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="O50" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="P50" s="22"/>
+      <c r="Q50" s="22"/>
+      <c r="R50" s="24"/>
+      <c r="S50" s="15"/>
+    </row>
+    <row r="51" spans="1:19" ht="60">
+      <c r="A51" s="19">
+        <f>A50+1</f>
+        <v>2</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" s="21"/>
+      <c r="E51" s="69" t="s">
+        <v>67</v>
+      </c>
+      <c r="F51" s="21"/>
+      <c r="G51" s="73"/>
+      <c r="H51" s="73"/>
+      <c r="I51" s="73"/>
+      <c r="J51" s="21">
+        <v>0</v>
+      </c>
+      <c r="K51" s="21"/>
+      <c r="L51" s="66"/>
+      <c r="M51" s="66"/>
+      <c r="N51" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="O51" s="21"/>
+      <c r="P51" s="22"/>
+      <c r="Q51" s="22"/>
+      <c r="R51" s="24"/>
+      <c r="S51" s="15"/>
+    </row>
+    <row r="52" spans="1:19">
+      <c r="A52" s="19">
+        <f t="shared" ref="A52:A54" si="0">A51+1</f>
+        <v>3</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="75" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="73" t="s">
-        <v>6</v>
-      </c>
-      <c r="G38" s="82" t="s">
-        <v>82</v>
-      </c>
-      <c r="H38" s="82" t="s">
-        <v>83</v>
-      </c>
-      <c r="I38" s="82" t="s">
-        <v>84</v>
-      </c>
-      <c r="J38" s="73" t="s">
-        <v>76</v>
-      </c>
-      <c r="K38" s="75" t="s">
-        <v>65</v>
-      </c>
-      <c r="L38" s="75" t="s">
-        <v>49</v>
-      </c>
-      <c r="M38" s="78" t="s">
-        <v>58</v>
-      </c>
-      <c r="N38" s="78" t="s">
-        <v>57</v>
-      </c>
-      <c r="O38" s="73" t="s">
-        <v>2</v>
-      </c>
-      <c r="P38" s="73"/>
-      <c r="Q38" s="16"/>
-      <c r="R38" s="17"/>
-      <c r="S38" s="9"/>
-    </row>
-    <row r="39" spans="1:19">
-      <c r="A39" s="74"/>
-      <c r="B39" s="74"/>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="76"/>
-      <c r="F39" s="73"/>
-      <c r="G39" s="82"/>
-      <c r="H39" s="82"/>
-      <c r="I39" s="82"/>
-      <c r="J39" s="73"/>
-      <c r="K39" s="77"/>
-      <c r="L39" s="77"/>
-      <c r="M39" s="79"/>
-      <c r="N39" s="79"/>
-      <c r="O39" s="73"/>
-      <c r="P39" s="73"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="25"/>
-      <c r="S39" s="15"/>
-    </row>
-    <row r="40" spans="1:19">
-      <c r="A40" s="19">
-        <v>1</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="F40" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="G40" s="83"/>
-      <c r="H40" s="83"/>
-      <c r="I40" s="83"/>
-      <c r="J40" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="K40" s="21"/>
-      <c r="L40" s="66"/>
-      <c r="M40" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="N40" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="O40" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="P40" s="22"/>
-      <c r="Q40" s="22"/>
-      <c r="R40" s="24"/>
-      <c r="S40" s="15"/>
-    </row>
-    <row r="41" spans="1:19" ht="60">
-      <c r="A41" s="19">
-        <f>A40+1</f>
-        <v>2</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D41" s="21"/>
-      <c r="E41" s="69" t="s">
-        <v>68</v>
-      </c>
-      <c r="F41" s="21"/>
-      <c r="G41" s="84"/>
-      <c r="H41" s="84"/>
-      <c r="I41" s="84"/>
-      <c r="J41" s="21">
-        <v>0</v>
-      </c>
-      <c r="K41" s="21"/>
-      <c r="L41" s="66"/>
-      <c r="M41" s="66"/>
-      <c r="N41" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="O41" s="21"/>
-      <c r="P41" s="22"/>
-      <c r="Q41" s="22"/>
-      <c r="R41" s="24"/>
-      <c r="S41" s="15"/>
-    </row>
-    <row r="42" spans="1:19">
-      <c r="A42" s="19">
-        <f t="shared" ref="A42:A44" si="0">A41+1</f>
-        <v>3</v>
-      </c>
-      <c r="B42" s="20" t="s">
+      <c r="E52" s="21"/>
+      <c r="F52" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G52" s="73"/>
+      <c r="H52" s="73"/>
+      <c r="I52" s="73"/>
+      <c r="J52" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="K52" s="21"/>
+      <c r="L52" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="M52" s="66"/>
+      <c r="N52" s="66"/>
+      <c r="O52" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="G42" s="84"/>
-      <c r="H42" s="84"/>
-      <c r="I42" s="84"/>
-      <c r="J42" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="K42" s="21"/>
-      <c r="L42" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="M42" s="66"/>
-      <c r="N42" s="66"/>
-      <c r="O42" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="P42" s="22"/>
-      <c r="Q42" s="22"/>
-      <c r="R42" s="23"/>
-      <c r="S42" s="15"/>
-    </row>
-    <row r="43" spans="1:19" ht="30">
-      <c r="A43" s="19">
+      <c r="P52" s="22"/>
+      <c r="Q52" s="22"/>
+      <c r="R52" s="23"/>
+      <c r="S52" s="15"/>
+    </row>
+    <row r="53" spans="1:19" ht="30">
+      <c r="A53" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B53" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D53" s="21"/>
+      <c r="E53" s="69" t="s">
+        <v>65</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G53" s="73"/>
+      <c r="H53" s="73"/>
+      <c r="I53" s="73"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="21"/>
+      <c r="L53" s="66"/>
+      <c r="M53" s="66"/>
+      <c r="N53" s="66"/>
+      <c r="O53" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D43" s="21"/>
-      <c r="E43" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="F43" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="G43" s="84"/>
-      <c r="H43" s="84"/>
-      <c r="I43" s="84"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21"/>
-      <c r="L43" s="66"/>
-      <c r="M43" s="66"/>
-      <c r="N43" s="66"/>
-      <c r="O43" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="P43" s="22"/>
-      <c r="Q43" s="22"/>
-      <c r="R43" s="23"/>
-      <c r="S43" s="15"/>
-    </row>
-    <row r="44" spans="1:19" ht="15">
-      <c r="A44" s="19">
+      <c r="P53" s="22"/>
+      <c r="Q53" s="22"/>
+      <c r="R53" s="23"/>
+      <c r="S53" s="15"/>
+    </row>
+    <row r="54" spans="1:19" ht="15">
+      <c r="A54" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B44" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="21"/>
-      <c r="E44" s="67" t="s">
-        <v>69</v>
-      </c>
-      <c r="F44" s="21"/>
-      <c r="G44" s="85"/>
-      <c r="H44" s="85"/>
-      <c r="I44" s="85"/>
-      <c r="J44" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="K44" s="21"/>
-      <c r="L44" s="66"/>
-      <c r="M44" s="66"/>
-      <c r="N44" s="66"/>
-      <c r="O44" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="P44" s="22"/>
-      <c r="Q44" s="22"/>
-      <c r="R44" s="23"/>
-      <c r="S44" s="15"/>
-    </row>
-    <row r="45" spans="1:19">
-      <c r="A45" s="103">
+      <c r="B54" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54" s="21"/>
+      <c r="E54" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="F54" s="21"/>
+      <c r="G54" s="74"/>
+      <c r="H54" s="74"/>
+      <c r="I54" s="74"/>
+      <c r="J54" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="K54" s="21"/>
+      <c r="L54" s="66"/>
+      <c r="M54" s="66"/>
+      <c r="N54" s="66"/>
+      <c r="O54" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="P54" s="22"/>
+      <c r="Q54" s="22"/>
+      <c r="R54" s="23"/>
+      <c r="S54" s="15"/>
+    </row>
+    <row r="55" spans="1:19" ht="30">
+      <c r="A55" s="92">
         <v>6</v>
       </c>
-      <c r="B45" s="104" t="s">
+      <c r="B55" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="E55" s="21"/>
+      <c r="F55" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="G45" s="84" t="s">
+      <c r="G55" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="H55" s="73"/>
+      <c r="I55" s="69" t="s">
+        <v>93</v>
+      </c>
+      <c r="J55" s="21"/>
+      <c r="K55" s="21"/>
+      <c r="L55" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="M55" s="66"/>
+      <c r="N55" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="O55" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="H45" s="84"/>
-      <c r="I45" s="85" t="s">
-        <v>86</v>
-      </c>
-      <c r="J45" s="21"/>
-      <c r="K45" s="21"/>
-      <c r="L45" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="M45" s="66"/>
-      <c r="N45" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="O45" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="P45" s="22"/>
-      <c r="Q45" s="22"/>
-      <c r="R45" s="23"/>
-      <c r="S45" s="15"/>
-    </row>
-    <row r="46" spans="1:19">
-      <c r="A46" s="97"/>
-      <c r="B46" s="98"/>
-      <c r="C46" s="99"/>
-      <c r="D46" s="99"/>
-      <c r="E46" s="99"/>
-      <c r="F46" s="99"/>
-      <c r="G46" s="106"/>
-      <c r="H46" s="107"/>
-      <c r="I46" s="107"/>
-      <c r="J46" s="99"/>
-      <c r="K46" s="99"/>
-      <c r="L46" s="100"/>
-      <c r="M46" s="100"/>
-      <c r="N46" s="100"/>
-      <c r="O46" s="99"/>
-      <c r="P46" s="101"/>
-      <c r="Q46" s="101"/>
-      <c r="R46" s="102"/>
-      <c r="S46" s="15"/>
-    </row>
-    <row r="47" spans="1:19">
-      <c r="G47" s="41"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="41"/>
-    </row>
-    <row r="48" spans="1:19">
-      <c r="G48" s="105"/>
-      <c r="H48" s="105"/>
-      <c r="I48" s="105"/>
-    </row>
-    <row r="49" spans="7:9">
-      <c r="G49" s="41"/>
-      <c r="H49" s="41"/>
-      <c r="I49" s="41"/>
-    </row>
-    <row r="50" spans="7:9">
-      <c r="G50" s="41"/>
-      <c r="H50" s="41"/>
-      <c r="I50" s="41"/>
-    </row>
-    <row r="51" spans="7:9">
-      <c r="G51" s="41"/>
-      <c r="H51" s="41"/>
-      <c r="I51" s="41"/>
-    </row>
-    <row r="52" spans="7:9">
-      <c r="G52" s="41"/>
-      <c r="H52" s="41"/>
-      <c r="I52" s="41"/>
-    </row>
-    <row r="53" spans="7:9">
-      <c r="G53" s="41"/>
-      <c r="H53" s="41"/>
-      <c r="I53" s="41"/>
-    </row>
-    <row r="54" spans="7:9">
-      <c r="G54" s="41"/>
-      <c r="H54" s="41"/>
-      <c r="I54" s="41"/>
+      <c r="P55" s="22"/>
+      <c r="Q55" s="22"/>
+      <c r="R55" s="23"/>
+      <c r="S55" s="15"/>
+    </row>
+    <row r="56" spans="1:19">
+      <c r="A56" s="86"/>
+      <c r="B56" s="87"/>
+      <c r="C56" s="88"/>
+      <c r="D56" s="88"/>
+      <c r="E56" s="88"/>
+      <c r="F56" s="88"/>
+      <c r="G56" s="95"/>
+      <c r="H56" s="96"/>
+      <c r="I56" s="96"/>
+      <c r="J56" s="88"/>
+      <c r="K56" s="88"/>
+      <c r="L56" s="89"/>
+      <c r="M56" s="89"/>
+      <c r="N56" s="89"/>
+      <c r="O56" s="88"/>
+      <c r="P56" s="90"/>
+      <c r="Q56" s="90"/>
+      <c r="R56" s="91"/>
+      <c r="S56" s="15"/>
+    </row>
+    <row r="57" spans="1:19">
+      <c r="G57" s="41"/>
+      <c r="H57" s="41"/>
+      <c r="I57" s="41"/>
+    </row>
+    <row r="58" spans="1:19">
+      <c r="G58" s="94"/>
+      <c r="H58" s="94"/>
+      <c r="I58" s="94"/>
+    </row>
+    <row r="59" spans="1:19">
+      <c r="G59" s="41"/>
+      <c r="H59" s="41"/>
+      <c r="I59" s="41"/>
+    </row>
+    <row r="60" spans="1:19">
+      <c r="G60" s="41"/>
+      <c r="H60" s="41"/>
+      <c r="I60" s="41"/>
+    </row>
+    <row r="61" spans="1:19">
+      <c r="G61" s="41"/>
+      <c r="H61" s="41"/>
+      <c r="I61" s="41"/>
+    </row>
+    <row r="62" spans="1:19">
+      <c r="G62" s="41"/>
+      <c r="H62" s="41"/>
+      <c r="I62" s="41"/>
+    </row>
+    <row r="63" spans="1:19">
+      <c r="G63" s="41"/>
+      <c r="H63" s="41"/>
+      <c r="I63" s="41"/>
+    </row>
+    <row r="64" spans="1:19">
+      <c r="G64" s="41"/>
+      <c r="H64" s="41"/>
+      <c r="I64" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="22">
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
     <mergeCell ref="C11:F11"/>
-    <mergeCell ref="O38:P39"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="N38:N39"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="K38:K39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="O48:P49"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="L48:L49"/>
+    <mergeCell ref="N48:N49"/>
+    <mergeCell ref="M48:M49"/>
+    <mergeCell ref="K48:K49"/>
+    <mergeCell ref="J48:J49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="H48:H49"/>
+    <mergeCell ref="I48:I49"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F62 J62:N62" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F72 J72:N72" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2893,7 +3146,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15 K40:K46" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15 K50:K56" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>isAbstract</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{061A2328-C320-074B-A7A0-1D5ADA23E625}">
@@ -2915,7 +3168,7 @@
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>
           </x14:formula1>
-          <xm:sqref>L40:N46</xm:sqref>
+          <xm:sqref>L50:N56</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2931,7 +3184,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -2954,7 +3207,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="19">
       <c r="A1" s="49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -2969,43 +3222,43 @@
       <c r="L1" s="49"/>
       <c r="M1" s="49"/>
       <c r="N1" s="50" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q1" s="50"/>
     </row>
     <row r="3" spans="1:17">
       <c r="B3" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="52" t="s">
+      <c r="J3" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="52" t="s">
+      <c r="L3" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="52" t="s">
+      <c r="N3" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="52" t="s">
-        <v>41</v>
-      </c>
       <c r="P3" s="52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="B4" s="53"/>
       <c r="D4" s="56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H4" s="54"/>
       <c r="J4" s="54"/>
@@ -3015,24 +3268,24 @@
     </row>
     <row r="5" spans="1:17">
       <c r="B5" s="55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="56"/>
       <c r="F5" s="56"/>
       <c r="H5" s="56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J5" s="56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L5" s="56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N5" s="56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P5" s="56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:17">

</xml_diff>

<commit_message>
0.0.13: Remove line terminator semi-colon from toString method.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D60BDF-5A60-2B43-B765-F1A9FC02D31A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223CD6F9-111C-4546-93FC-2E570A540EAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="2220" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6860" yWindow="1180" windowWidth="25440" windowHeight="18580" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
   <si>
     <t>クラス名</t>
   </si>
@@ -1876,8 +1876,8 @@
   </sheetPr>
   <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2169,7 +2169,9 @@
         <v>43</v>
       </c>
       <c r="B17" s="59"/>
-      <c r="C17" s="60"/>
+      <c r="C17" s="60" t="s">
+        <v>44</v>
+      </c>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>

</xml_diff>

<commit_message>
0.0.14: * force data class to final, if not specified.         * integer should be converted to kotlin.Long.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223CD6F9-111C-4546-93FC-2E570A540EAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE146427-067F-9447-A8D5-B5D11DA28C77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6860" yWindow="1180" windowWidth="25440" windowHeight="18580" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="96">
   <si>
     <t>クラス名</t>
   </si>
@@ -536,6 +536,23 @@
   <si>
     <t>@JsonProperty
 @hoge</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>intArray</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>総称型のintegerがLongに変換されることを確認します。</t>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">ソウショウガタ </t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t xml:space="preserve">ヘンカｎ </t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t xml:space="preserve">カクニｎ </t>
+    </rPh>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1242,7 +1259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1409,46 +1426,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1458,11 +1439,44 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1874,10 +1888,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S64"/>
+  <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="F27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O57" sqref="O57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2043,12 +2057,12 @@
         <v>2</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="97" t="s">
+      <c r="C11" s="106" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="98"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="99"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="108"/>
       <c r="H11" s="40"/>
       <c r="I11" s="40"/>
       <c r="J11" s="61"/>
@@ -2148,9 +2162,7 @@
         <v>60</v>
       </c>
       <c r="B16" s="59"/>
-      <c r="C16" s="60" t="s">
-        <v>44</v>
-      </c>
+      <c r="C16" s="60"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
@@ -2453,32 +2465,32 @@
       <c r="Q30" s="33"/>
     </row>
     <row r="31" spans="1:19" s="28" customFormat="1">
-      <c r="A31" s="108" t="s">
+      <c r="A31" s="96" t="s">
         <v>86</v>
       </c>
       <c r="B31" s="59"/>
       <c r="C31" s="59"/>
       <c r="D31" s="59"/>
       <c r="E31" s="59"/>
-      <c r="F31" s="109"/>
+      <c r="F31" s="97"/>
     </row>
     <row r="32" spans="1:19" s="28" customFormat="1">
-      <c r="A32" s="101" t="s">
+      <c r="A32" s="104" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="101" t="s">
+      <c r="B32" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="107" t="s">
+      <c r="C32" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="107" t="s">
+      <c r="D32" s="105" t="s">
         <v>88</v>
       </c>
-      <c r="E32" s="107" t="s">
+      <c r="E32" s="105" t="s">
         <v>89</v>
       </c>
-      <c r="F32" s="113"/>
+      <c r="F32" s="103"/>
       <c r="G32" s="70"/>
       <c r="H32" s="70"/>
       <c r="I32" s="70"/>
@@ -2486,12 +2498,12 @@
       <c r="K32" s="70"/>
     </row>
     <row r="33" spans="1:19" s="28" customFormat="1">
-      <c r="A33" s="101"/>
-      <c r="B33" s="101"/>
-      <c r="C33" s="107"/>
-      <c r="D33" s="107"/>
-      <c r="E33" s="107"/>
-      <c r="F33" s="113"/>
+      <c r="A33" s="104"/>
+      <c r="B33" s="104"/>
+      <c r="C33" s="105"/>
+      <c r="D33" s="105"/>
+      <c r="E33" s="105"/>
+      <c r="F33" s="103"/>
       <c r="G33" s="70"/>
       <c r="H33" s="70"/>
       <c r="I33" s="70"/>
@@ -2514,7 +2526,7 @@
       <c r="E34" s="73" t="s">
         <v>91</v>
       </c>
-      <c r="F34" s="114"/>
+      <c r="F34" s="101"/>
       <c r="G34" s="70"/>
       <c r="H34" s="70"/>
       <c r="I34" s="70"/>
@@ -2528,7 +2540,7 @@
       <c r="C35" s="73"/>
       <c r="D35" s="73"/>
       <c r="E35" s="73"/>
-      <c r="F35" s="114"/>
+      <c r="F35" s="101"/>
       <c r="G35" s="70"/>
       <c r="H35" s="70"/>
       <c r="I35" s="70"/>
@@ -2542,7 +2554,7 @@
       <c r="C36" s="73"/>
       <c r="D36" s="73"/>
       <c r="E36" s="73"/>
-      <c r="F36" s="114"/>
+      <c r="F36" s="101"/>
       <c r="G36" s="70"/>
       <c r="H36" s="70"/>
       <c r="I36" s="70"/>
@@ -2556,7 +2568,7 @@
       <c r="C37" s="73"/>
       <c r="D37" s="73"/>
       <c r="E37" s="73"/>
-      <c r="F37" s="114"/>
+      <c r="F37" s="101"/>
       <c r="G37" s="70"/>
       <c r="H37" s="70"/>
       <c r="I37" s="70"/>
@@ -2570,7 +2582,7 @@
       <c r="C38" s="73"/>
       <c r="D38" s="73"/>
       <c r="E38" s="73"/>
-      <c r="F38" s="114"/>
+      <c r="F38" s="101"/>
       <c r="G38" s="70"/>
       <c r="H38" s="70"/>
       <c r="I38" s="70"/>
@@ -2579,12 +2591,12 @@
       <c r="L38" s="70"/>
     </row>
     <row r="39" spans="1:19" s="28" customFormat="1">
-      <c r="A39" s="110"/>
-      <c r="B39" s="111"/>
-      <c r="C39" s="112"/>
-      <c r="D39" s="112"/>
-      <c r="E39" s="112"/>
-      <c r="F39" s="115"/>
+      <c r="A39" s="98"/>
+      <c r="B39" s="99"/>
+      <c r="C39" s="100"/>
+      <c r="D39" s="100"/>
+      <c r="E39" s="100"/>
+      <c r="F39" s="102"/>
       <c r="G39" s="70"/>
       <c r="H39" s="70"/>
       <c r="I39" s="70"/>
@@ -2756,73 +2768,73 @@
       <c r="S47" s="15"/>
     </row>
     <row r="48" spans="1:19" ht="13.5" customHeight="1">
-      <c r="A48" s="101" t="s">
+      <c r="A48" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="B48" s="101" t="s">
+      <c r="B48" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="100" t="s">
+      <c r="C48" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="100" t="s">
+      <c r="D48" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="E48" s="102" t="s">
+      <c r="E48" s="110" t="s">
         <v>22</v>
       </c>
-      <c r="F48" s="100" t="s">
+      <c r="F48" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="107" t="s">
+      <c r="G48" s="105" t="s">
         <v>81</v>
       </c>
-      <c r="H48" s="107" t="s">
+      <c r="H48" s="105" t="s">
         <v>82</v>
       </c>
-      <c r="I48" s="107" t="s">
+      <c r="I48" s="105" t="s">
         <v>83</v>
       </c>
-      <c r="J48" s="100" t="s">
+      <c r="J48" s="109" t="s">
         <v>75</v>
       </c>
-      <c r="K48" s="102" t="s">
+      <c r="K48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="L48" s="102" t="s">
+      <c r="L48" s="110" t="s">
         <v>48</v>
       </c>
-      <c r="M48" s="105" t="s">
+      <c r="M48" s="113" t="s">
         <v>57</v>
       </c>
-      <c r="N48" s="105" t="s">
+      <c r="N48" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="O48" s="100" t="s">
+      <c r="O48" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="P48" s="100"/>
+      <c r="P48" s="109"/>
       <c r="Q48" s="16"/>
       <c r="R48" s="17"/>
       <c r="S48" s="9"/>
     </row>
     <row r="49" spans="1:19">
-      <c r="A49" s="101"/>
-      <c r="B49" s="101"/>
-      <c r="C49" s="100"/>
-      <c r="D49" s="100"/>
-      <c r="E49" s="103"/>
-      <c r="F49" s="100"/>
-      <c r="G49" s="107"/>
-      <c r="H49" s="107"/>
-      <c r="I49" s="107"/>
-      <c r="J49" s="100"/>
-      <c r="K49" s="104"/>
-      <c r="L49" s="104"/>
-      <c r="M49" s="106"/>
-      <c r="N49" s="106"/>
-      <c r="O49" s="100"/>
-      <c r="P49" s="100"/>
+      <c r="A49" s="104"/>
+      <c r="B49" s="104"/>
+      <c r="C49" s="109"/>
+      <c r="D49" s="109"/>
+      <c r="E49" s="111"/>
+      <c r="F49" s="109"/>
+      <c r="G49" s="105"/>
+      <c r="H49" s="105"/>
+      <c r="I49" s="105"/>
+      <c r="J49" s="109"/>
+      <c r="K49" s="112"/>
+      <c r="L49" s="112"/>
+      <c r="M49" s="114"/>
+      <c r="N49" s="114"/>
+      <c r="O49" s="109"/>
+      <c r="P49" s="109"/>
       <c r="Q49" s="18"/>
       <c r="R49" s="25"/>
       <c r="S49" s="15"/>
@@ -2902,7 +2914,7 @@
     </row>
     <row r="52" spans="1:19">
       <c r="A52" s="19">
-        <f t="shared" ref="A52:A54" si="0">A51+1</f>
+        <f t="shared" ref="A52:A56" si="0">A51+1</f>
         <v>3</v>
       </c>
       <c r="B52" s="20" t="s">
@@ -3007,10 +3019,11 @@
       <c r="S54" s="15"/>
     </row>
     <row r="55" spans="1:19" ht="30">
-      <c r="A55" s="92">
+      <c r="A55" s="19">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B55" s="93" t="s">
+      <c r="B55" s="92" t="s">
         <v>72</v>
       </c>
       <c r="C55" s="21" t="s">
@@ -3048,40 +3061,71 @@
       <c r="S55" s="15"/>
     </row>
     <row r="56" spans="1:19">
-      <c r="A56" s="86"/>
-      <c r="B56" s="87"/>
-      <c r="C56" s="88"/>
-      <c r="D56" s="88"/>
-      <c r="E56" s="88"/>
-      <c r="F56" s="88"/>
-      <c r="G56" s="95"/>
-      <c r="H56" s="96"/>
-      <c r="I56" s="96"/>
-      <c r="J56" s="88"/>
-      <c r="K56" s="88"/>
-      <c r="L56" s="89"/>
-      <c r="M56" s="89"/>
-      <c r="N56" s="89"/>
-      <c r="O56" s="88"/>
-      <c r="P56" s="90"/>
-      <c r="Q56" s="90"/>
-      <c r="R56" s="91"/>
+      <c r="A56" s="19">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B56" s="92" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="73"/>
+      <c r="H56" s="73"/>
+      <c r="I56" s="69"/>
+      <c r="J56" s="21"/>
+      <c r="K56" s="21"/>
+      <c r="L56" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="M56" s="66"/>
+      <c r="N56" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="O56" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="P56" s="22"/>
+      <c r="Q56" s="22"/>
+      <c r="R56" s="23"/>
       <c r="S56" s="15"/>
     </row>
     <row r="57" spans="1:19">
-      <c r="G57" s="41"/>
-      <c r="H57" s="41"/>
-      <c r="I57" s="41"/>
+      <c r="A57" s="86"/>
+      <c r="B57" s="87"/>
+      <c r="C57" s="88"/>
+      <c r="D57" s="88"/>
+      <c r="E57" s="88"/>
+      <c r="F57" s="88"/>
+      <c r="G57" s="94"/>
+      <c r="H57" s="95"/>
+      <c r="I57" s="95"/>
+      <c r="J57" s="88"/>
+      <c r="K57" s="88"/>
+      <c r="L57" s="89"/>
+      <c r="M57" s="89"/>
+      <c r="N57" s="89"/>
+      <c r="O57" s="88"/>
+      <c r="P57" s="90"/>
+      <c r="Q57" s="90"/>
+      <c r="R57" s="91"/>
+      <c r="S57" s="15"/>
     </row>
     <row r="58" spans="1:19">
-      <c r="G58" s="94"/>
-      <c r="H58" s="94"/>
-      <c r="I58" s="94"/>
+      <c r="G58" s="41"/>
+      <c r="H58" s="41"/>
+      <c r="I58" s="41"/>
     </row>
     <row r="59" spans="1:19">
-      <c r="G59" s="41"/>
-      <c r="H59" s="41"/>
-      <c r="I59" s="41"/>
+      <c r="G59" s="93"/>
+      <c r="H59" s="93"/>
+      <c r="I59" s="93"/>
     </row>
     <row r="60" spans="1:19">
       <c r="G60" s="41"/>
@@ -3108,14 +3152,13 @@
       <c r="H64" s="41"/>
       <c r="I64" s="41"/>
     </row>
+    <row r="65" spans="7:9">
+      <c r="G65" s="41"/>
+      <c r="H65" s="41"/>
+      <c r="I65" s="41"/>
+    </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="O48:P49"/>
     <mergeCell ref="A48:A49"/>
@@ -3132,10 +3175,16 @@
     <mergeCell ref="G48:G49"/>
     <mergeCell ref="H48:H49"/>
     <mergeCell ref="I48:I49"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F72 J72:N72" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F73 J73:N73" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3148,7 +3197,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15 K50:K56" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15 K50:K57" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>isAbstract</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{061A2328-C320-074B-A7A0-1D5ADA23E625}">
@@ -3170,7 +3219,7 @@
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>
           </x14:formula1>
-          <xm:sqref>L50:N56</xm:sqref>
+          <xm:sqref>L50:N57</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
0.1.1: search package improvement for generate extends.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE146427-067F-9447-A8D5-B5D11DA28C77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB08049-78FA-2B41-8682-8E50945DDB90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6860" yWindow="1180" windowWidth="25440" windowHeight="18580" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="98">
   <si>
     <t>クラス名</t>
   </si>
@@ -553,6 +553,14 @@
     <rPh sb="25" eb="27">
       <t xml:space="preserve">カクニｎ </t>
     </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>SimpleSample2</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>blanco.sample.valueobjectkt.simple</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1441,41 +1449,41 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1888,10 +1896,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S65"/>
+  <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O57" sqref="O57"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2057,12 +2065,12 @@
         <v>2</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="106" t="s">
+      <c r="C11" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="107"/>
-      <c r="E11" s="107"/>
-      <c r="F11" s="108"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="104"/>
+      <c r="F11" s="105"/>
       <c r="H11" s="40"/>
       <c r="I11" s="40"/>
       <c r="J11" s="61"/>
@@ -2264,7 +2272,9 @@
         <v>0</v>
       </c>
       <c r="B21" s="30"/>
-      <c r="C21" s="31"/>
+      <c r="C21" s="31" t="s">
+        <v>96</v>
+      </c>
       <c r="D21" s="31"/>
       <c r="E21" s="31"/>
       <c r="F21" s="79"/>
@@ -2287,7 +2297,9 @@
         <v>21</v>
       </c>
       <c r="B22" s="6"/>
-      <c r="C22" s="10"/>
+      <c r="C22" s="10" t="s">
+        <v>97</v>
+      </c>
       <c r="D22" s="32"/>
       <c r="E22" s="32"/>
       <c r="F22" s="80"/>
@@ -2320,15 +2332,18 @@
       <c r="O23" s="34"/>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="33"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="70"/>
-      <c r="H24" s="76"/>
-      <c r="I24" s="76"/>
+      <c r="A24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="81"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
       <c r="J24" s="33"/>
       <c r="K24" s="33"/>
       <c r="L24" s="33"/>
@@ -2337,84 +2352,80 @@
       <c r="O24" s="34"/>
     </row>
     <row r="25" spans="1:19">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="33"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="76"/>
+      <c r="I25" s="76"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="34"/>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="40"/>
-      <c r="Q25" s="40"/>
-      <c r="R25" s="40"/>
-      <c r="S25" s="40"/>
-    </row>
-    <row r="26" spans="1:19">
-      <c r="A26" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="82"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="78"/>
       <c r="G26" s="71"/>
       <c r="H26" s="77"/>
       <c r="I26" s="77"/>
-      <c r="J26" s="63"/>
-      <c r="K26" s="63"/>
-      <c r="L26" s="63"/>
-      <c r="M26" s="63"/>
-      <c r="N26" s="63"/>
-      <c r="O26" s="63"/>
-      <c r="P26" s="41"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="42"/>
-      <c r="S26" s="34"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="41"/>
+      <c r="L26" s="41"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="41"/>
+      <c r="P26" s="40"/>
+      <c r="Q26" s="40"/>
+      <c r="R26" s="40"/>
+      <c r="S26" s="40"/>
     </row>
     <row r="27" spans="1:19">
-      <c r="A27" s="47"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="83"/>
+      <c r="A27" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="82"/>
       <c r="G27" s="71"/>
       <c r="H27" s="77"/>
       <c r="I27" s="77"/>
-      <c r="J27" s="64"/>
-      <c r="K27" s="64"/>
-      <c r="L27" s="64"/>
-      <c r="M27" s="64"/>
-      <c r="N27" s="64"/>
-      <c r="O27" s="33"/>
-      <c r="P27" s="35"/>
-      <c r="Q27" s="35"/>
-      <c r="R27" s="35"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="63"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="63"/>
+      <c r="P27" s="41"/>
+      <c r="Q27" s="42"/>
+      <c r="R27" s="42"/>
       <c r="S27" s="34"/>
     </row>
     <row r="28" spans="1:19">
       <c r="A28" s="47"/>
       <c r="B28" s="43"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="84"/>
-      <c r="G28"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="75"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="83"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="77"/>
+      <c r="I28" s="77"/>
       <c r="J28" s="64"/>
       <c r="K28" s="64"/>
       <c r="L28" s="64"/>
@@ -2427,14 +2438,15 @@
       <c r="S28" s="34"/>
     </row>
     <row r="29" spans="1:19">
-      <c r="A29" s="48"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="85"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
+      <c r="A29" s="47"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="84"/>
+      <c r="G29"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="75"/>
       <c r="J29" s="64"/>
       <c r="K29" s="64"/>
       <c r="L29" s="64"/>
@@ -2446,64 +2458,71 @@
       <c r="R29" s="35"/>
       <c r="S29" s="34"/>
     </row>
-    <row r="30" spans="1:19" s="36" customFormat="1">
-      <c r="A30" s="33"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="33"/>
+    <row r="30" spans="1:19">
+      <c r="A30" s="48"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="85"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="64"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="64"/>
+      <c r="M30" s="64"/>
+      <c r="N30" s="64"/>
       <c r="O30" s="33"/>
-      <c r="P30" s="33"/>
-      <c r="Q30" s="33"/>
-    </row>
-    <row r="31" spans="1:19" s="28" customFormat="1">
-      <c r="A31" s="96" t="s">
+      <c r="P30" s="35"/>
+      <c r="Q30" s="35"/>
+      <c r="R30" s="35"/>
+      <c r="S30" s="34"/>
+    </row>
+    <row r="31" spans="1:19" s="36" customFormat="1">
+      <c r="A31" s="33"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="33"/>
+      <c r="O31" s="33"/>
+      <c r="P31" s="33"/>
+      <c r="Q31" s="33"/>
+    </row>
+    <row r="32" spans="1:19" s="28" customFormat="1">
+      <c r="A32" s="96" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="59"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="97"/>
-    </row>
-    <row r="32" spans="1:19" s="28" customFormat="1">
-      <c r="A32" s="104" t="s">
+      <c r="B32" s="59"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="97"/>
+    </row>
+    <row r="33" spans="1:19" s="28" customFormat="1">
+      <c r="A33" s="107" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="104" t="s">
+      <c r="B33" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="105" t="s">
+      <c r="C33" s="113" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="105" t="s">
+      <c r="D33" s="113" t="s">
         <v>88</v>
       </c>
-      <c r="E32" s="105" t="s">
+      <c r="E33" s="113" t="s">
         <v>89</v>
       </c>
-      <c r="F32" s="103"/>
-      <c r="G32" s="70"/>
-      <c r="H32" s="70"/>
-      <c r="I32" s="70"/>
-      <c r="J32" s="70"/>
-      <c r="K32" s="70"/>
-    </row>
-    <row r="33" spans="1:19" s="28" customFormat="1">
-      <c r="A33" s="104"/>
-      <c r="B33" s="104"/>
-      <c r="C33" s="105"/>
-      <c r="D33" s="105"/>
-      <c r="E33" s="105"/>
-      <c r="F33" s="103"/>
+      <c r="F33" s="114"/>
       <c r="G33" s="70"/>
       <c r="H33" s="70"/>
       <c r="I33" s="70"/>
@@ -2511,35 +2530,34 @@
       <c r="K33" s="70"/>
     </row>
     <row r="34" spans="1:19" s="28" customFormat="1">
-      <c r="A34" s="19">
-        <v>1</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="73" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" s="73" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" s="73" t="s">
-        <v>91</v>
-      </c>
-      <c r="F34" s="101"/>
+      <c r="A34" s="107"/>
+      <c r="B34" s="107"/>
+      <c r="C34" s="113"/>
+      <c r="D34" s="113"/>
+      <c r="E34" s="113"/>
+      <c r="F34" s="114"/>
       <c r="G34" s="70"/>
       <c r="H34" s="70"/>
       <c r="I34" s="70"/>
       <c r="J34" s="70"/>
       <c r="K34" s="70"/>
-      <c r="L34" s="70"/>
     </row>
     <row r="35" spans="1:19" s="28" customFormat="1">
-      <c r="A35" s="19"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="73"/>
-      <c r="D35" s="73"/>
-      <c r="E35" s="73"/>
+      <c r="A35" s="19">
+        <v>1</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="73" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="73" t="s">
+        <v>91</v>
+      </c>
       <c r="F35" s="101"/>
       <c r="G35" s="70"/>
       <c r="H35" s="70"/>
@@ -2591,12 +2609,12 @@
       <c r="L38" s="70"/>
     </row>
     <row r="39" spans="1:19" s="28" customFormat="1">
-      <c r="A39" s="98"/>
-      <c r="B39" s="99"/>
-      <c r="C39" s="100"/>
-      <c r="D39" s="100"/>
-      <c r="E39" s="100"/>
-      <c r="F39" s="102"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="101"/>
       <c r="G39" s="70"/>
       <c r="H39" s="70"/>
       <c r="I39" s="70"/>
@@ -2605,97 +2623,91 @@
       <c r="L39" s="70"/>
     </row>
     <row r="40" spans="1:19" s="28" customFormat="1">
-      <c r="A40"/>
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40"/>
-      <c r="I40"/>
-      <c r="J40"/>
-      <c r="K40"/>
-      <c r="L40" s="71"/>
-      <c r="M40"/>
-    </row>
-    <row r="41" spans="1:19">
-      <c r="A41" s="26" t="s">
+      <c r="A40" s="98"/>
+      <c r="B40" s="99"/>
+      <c r="C40" s="100"/>
+      <c r="D40" s="100"/>
+      <c r="E40" s="100"/>
+      <c r="F40" s="102"/>
+      <c r="G40" s="70"/>
+      <c r="H40" s="70"/>
+      <c r="I40" s="70"/>
+      <c r="J40" s="70"/>
+      <c r="K40" s="70"/>
+      <c r="L40" s="70"/>
+    </row>
+    <row r="41" spans="1:19" s="28" customFormat="1">
+      <c r="A41"/>
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41" s="71"/>
+      <c r="M41"/>
+    </row>
+    <row r="42" spans="1:19">
+      <c r="A42" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="78"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="40"/>
-      <c r="J41" s="41"/>
-      <c r="K41" s="41"/>
-      <c r="L41" s="41"/>
-      <c r="M41" s="41"/>
-      <c r="N41" s="41"/>
-      <c r="O41" s="41"/>
-      <c r="P41" s="40"/>
-      <c r="Q41" s="40"/>
-      <c r="R41" s="40"/>
-      <c r="S41" s="40"/>
-    </row>
-    <row r="42" spans="1:19">
-      <c r="A42" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="B42" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="82"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="78"/>
       <c r="H42" s="40"/>
       <c r="I42" s="40"/>
-      <c r="J42" s="63"/>
-      <c r="K42" s="63"/>
-      <c r="L42" s="63"/>
-      <c r="M42" s="63"/>
-      <c r="N42" s="63"/>
-      <c r="O42" s="63"/>
-      <c r="P42" s="41"/>
-      <c r="Q42" s="42"/>
-      <c r="R42" s="42"/>
-      <c r="S42" s="34"/>
+      <c r="J42" s="41"/>
+      <c r="K42" s="41"/>
+      <c r="L42" s="41"/>
+      <c r="M42" s="41"/>
+      <c r="N42" s="41"/>
+      <c r="O42" s="41"/>
+      <c r="P42" s="40"/>
+      <c r="Q42" s="40"/>
+      <c r="R42" s="40"/>
+      <c r="S42" s="40"/>
     </row>
     <row r="43" spans="1:19">
-      <c r="A43" s="47">
-        <v>1</v>
-      </c>
-      <c r="B43" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="83"/>
+      <c r="A43" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="82"/>
       <c r="H43" s="40"/>
       <c r="I43" s="40"/>
-      <c r="J43" s="64"/>
-      <c r="K43" s="64"/>
-      <c r="L43" s="64"/>
-      <c r="M43" s="64"/>
-      <c r="N43" s="64"/>
-      <c r="O43" s="33"/>
-      <c r="P43" s="35"/>
-      <c r="Q43" s="35"/>
-      <c r="R43" s="35"/>
+      <c r="J43" s="63"/>
+      <c r="K43" s="63"/>
+      <c r="L43" s="63"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="63"/>
+      <c r="O43" s="63"/>
+      <c r="P43" s="41"/>
+      <c r="Q43" s="42"/>
+      <c r="R43" s="42"/>
       <c r="S43" s="34"/>
     </row>
     <row r="44" spans="1:19">
-      <c r="A44" s="47"/>
-      <c r="B44" s="43"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="84"/>
+      <c r="A44" s="47">
+        <v>1</v>
+      </c>
+      <c r="B44" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="83"/>
       <c r="H44" s="40"/>
       <c r="I44" s="40"/>
       <c r="J44" s="64"/>
@@ -2710,12 +2722,12 @@
       <c r="S44" s="34"/>
     </row>
     <row r="45" spans="1:19">
-      <c r="A45" s="48"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="85"/>
+      <c r="A45" s="47"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="84"/>
       <c r="H45" s="40"/>
       <c r="I45" s="40"/>
       <c r="J45" s="64"/>
@@ -2730,355 +2742,339 @@
       <c r="S45" s="34"/>
     </row>
     <row r="46" spans="1:19">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="13"/>
-      <c r="O46" s="13"/>
-      <c r="P46" s="13"/>
+      <c r="A46" s="48"/>
+      <c r="B46" s="45"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="85"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="40"/>
+      <c r="J46" s="64"/>
+      <c r="K46" s="64"/>
+      <c r="L46" s="64"/>
+      <c r="M46" s="64"/>
+      <c r="N46" s="64"/>
+      <c r="O46" s="33"/>
+      <c r="P46" s="35"/>
+      <c r="Q46" s="35"/>
+      <c r="R46" s="35"/>
+      <c r="S46" s="34"/>
     </row>
     <row r="47" spans="1:19">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
+      <c r="P47" s="13"/>
+    </row>
+    <row r="48" spans="1:19">
+      <c r="A48" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="59"/>
-      <c r="H47" s="59"/>
-      <c r="I47" s="59"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="14"/>
-      <c r="O47" s="14"/>
-      <c r="P47" s="14"/>
-      <c r="Q47" s="14"/>
-      <c r="R47" s="6"/>
-      <c r="S47" s="15"/>
-    </row>
-    <row r="48" spans="1:19" ht="13.5" customHeight="1">
-      <c r="A48" s="104" t="s">
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="59"/>
+      <c r="H48" s="59"/>
+      <c r="I48" s="59"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="6"/>
+      <c r="S48" s="15"/>
+    </row>
+    <row r="49" spans="1:19" ht="13.5" customHeight="1">
+      <c r="A49" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B48" s="104" t="s">
+      <c r="B49" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="109" t="s">
+      <c r="C49" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="109" t="s">
+      <c r="D49" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="E48" s="110" t="s">
+      <c r="E49" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="F48" s="109" t="s">
+      <c r="F49" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="105" t="s">
+      <c r="G49" s="113" t="s">
         <v>81</v>
       </c>
-      <c r="H48" s="105" t="s">
+      <c r="H49" s="113" t="s">
         <v>82</v>
       </c>
-      <c r="I48" s="105" t="s">
+      <c r="I49" s="113" t="s">
         <v>83</v>
       </c>
-      <c r="J48" s="109" t="s">
+      <c r="J49" s="106" t="s">
         <v>75</v>
       </c>
-      <c r="K48" s="110" t="s">
+      <c r="K49" s="108" t="s">
         <v>64</v>
       </c>
-      <c r="L48" s="110" t="s">
+      <c r="L49" s="108" t="s">
         <v>48</v>
       </c>
-      <c r="M48" s="113" t="s">
+      <c r="M49" s="111" t="s">
         <v>57</v>
       </c>
-      <c r="N48" s="113" t="s">
+      <c r="N49" s="111" t="s">
         <v>56</v>
       </c>
-      <c r="O48" s="109" t="s">
+      <c r="O49" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="P48" s="109"/>
-      <c r="Q48" s="16"/>
-      <c r="R48" s="17"/>
-      <c r="S48" s="9"/>
-    </row>
-    <row r="49" spans="1:19">
-      <c r="A49" s="104"/>
-      <c r="B49" s="104"/>
-      <c r="C49" s="109"/>
-      <c r="D49" s="109"/>
-      <c r="E49" s="111"/>
-      <c r="F49" s="109"/>
-      <c r="G49" s="105"/>
-      <c r="H49" s="105"/>
-      <c r="I49" s="105"/>
-      <c r="J49" s="109"/>
-      <c r="K49" s="112"/>
-      <c r="L49" s="112"/>
-      <c r="M49" s="114"/>
-      <c r="N49" s="114"/>
-      <c r="O49" s="109"/>
-      <c r="P49" s="109"/>
-      <c r="Q49" s="18"/>
-      <c r="R49" s="25"/>
-      <c r="S49" s="15"/>
+      <c r="P49" s="106"/>
+      <c r="Q49" s="16"/>
+      <c r="R49" s="17"/>
+      <c r="S49" s="9"/>
     </row>
     <row r="50" spans="1:19">
-      <c r="A50" s="19">
+      <c r="A50" s="107"/>
+      <c r="B50" s="107"/>
+      <c r="C50" s="106"/>
+      <c r="D50" s="106"/>
+      <c r="E50" s="109"/>
+      <c r="F50" s="106"/>
+      <c r="G50" s="113"/>
+      <c r="H50" s="113"/>
+      <c r="I50" s="113"/>
+      <c r="J50" s="106"/>
+      <c r="K50" s="110"/>
+      <c r="L50" s="110"/>
+      <c r="M50" s="112"/>
+      <c r="N50" s="112"/>
+      <c r="O50" s="106"/>
+      <c r="P50" s="106"/>
+      <c r="Q50" s="18"/>
+      <c r="R50" s="25"/>
+      <c r="S50" s="15"/>
+    </row>
+    <row r="51" spans="1:19">
+      <c r="A51" s="19">
         <v>1</v>
       </c>
-      <c r="B50" s="20" t="s">
+      <c r="B51" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="21" t="s">
+      <c r="C51" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21" t="s">
+      <c r="D51" s="21"/>
+      <c r="E51" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F50" s="21" t="s">
+      <c r="F51" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G50" s="72"/>
-      <c r="H50" s="72"/>
-      <c r="I50" s="72"/>
-      <c r="J50" s="21" t="s">
+      <c r="G51" s="72"/>
+      <c r="H51" s="72"/>
+      <c r="I51" s="72"/>
+      <c r="J51" s="21" t="s">
         <v>76</v>
-      </c>
-      <c r="K50" s="21"/>
-      <c r="L50" s="66"/>
-      <c r="M50" s="66" t="s">
-        <v>44</v>
-      </c>
-      <c r="N50" s="66" t="s">
-        <v>44</v>
-      </c>
-      <c r="O50" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="P50" s="22"/>
-      <c r="Q50" s="22"/>
-      <c r="R50" s="24"/>
-      <c r="S50" s="15"/>
-    </row>
-    <row r="51" spans="1:19" ht="60">
-      <c r="A51" s="19">
-        <f>A50+1</f>
-        <v>2</v>
-      </c>
-      <c r="B51" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D51" s="21"/>
-      <c r="E51" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="F51" s="21"/>
-      <c r="G51" s="73"/>
-      <c r="H51" s="73"/>
-      <c r="I51" s="73"/>
-      <c r="J51" s="21">
-        <v>0</v>
       </c>
       <c r="K51" s="21"/>
       <c r="L51" s="66"/>
-      <c r="M51" s="66"/>
+      <c r="M51" s="66" t="s">
+        <v>44</v>
+      </c>
       <c r="N51" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="O51" s="21"/>
+      <c r="O51" s="21" t="s">
+        <v>13</v>
+      </c>
       <c r="P51" s="22"/>
       <c r="Q51" s="22"/>
       <c r="R51" s="24"/>
       <c r="S51" s="15"/>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:19" ht="60">
       <c r="A52" s="19">
-        <f t="shared" ref="A52:A56" si="0">A51+1</f>
-        <v>3</v>
+        <f>A51+1</f>
+        <v>2</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D52" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21" t="s">
-        <v>79</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="D52" s="21"/>
+      <c r="E52" s="69" t="s">
+        <v>67</v>
+      </c>
+      <c r="F52" s="21"/>
       <c r="G52" s="73"/>
       <c r="H52" s="73"/>
       <c r="I52" s="73"/>
-      <c r="J52" s="21" t="s">
-        <v>78</v>
+      <c r="J52" s="21">
+        <v>0</v>
       </c>
       <c r="K52" s="21"/>
-      <c r="L52" s="66" t="s">
+      <c r="L52" s="66"/>
+      <c r="M52" s="66"/>
+      <c r="N52" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="M52" s="66"/>
-      <c r="N52" s="66"/>
-      <c r="O52" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="O52" s="21"/>
       <c r="P52" s="22"/>
       <c r="Q52" s="22"/>
-      <c r="R52" s="23"/>
+      <c r="R52" s="24"/>
       <c r="S52" s="15"/>
     </row>
-    <row r="53" spans="1:19" ht="30">
+    <row r="53" spans="1:19">
       <c r="A53" s="19">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" ref="A53:A57" si="0">A52+1</f>
+        <v>3</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D53" s="21"/>
-      <c r="E53" s="69" t="s">
-        <v>65</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="21"/>
       <c r="F53" s="21" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G53" s="73"/>
       <c r="H53" s="73"/>
       <c r="I53" s="73"/>
-      <c r="J53" s="21"/>
+      <c r="J53" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="K53" s="21"/>
-      <c r="L53" s="66"/>
+      <c r="L53" s="66" t="s">
+        <v>44</v>
+      </c>
       <c r="M53" s="66"/>
       <c r="N53" s="66"/>
       <c r="O53" s="21" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="P53" s="22"/>
       <c r="Q53" s="22"/>
       <c r="R53" s="23"/>
       <c r="S53" s="15"/>
     </row>
-    <row r="54" spans="1:19" ht="15">
+    <row r="54" spans="1:19" ht="30">
       <c r="A54" s="19">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D54" s="21"/>
-      <c r="E54" s="67" t="s">
-        <v>68</v>
-      </c>
-      <c r="F54" s="21"/>
-      <c r="G54" s="74"/>
-      <c r="H54" s="74"/>
-      <c r="I54" s="74"/>
-      <c r="J54" s="21" t="s">
-        <v>80</v>
-      </c>
+      <c r="E54" s="69" t="s">
+        <v>65</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G54" s="73"/>
+      <c r="H54" s="73"/>
+      <c r="I54" s="73"/>
+      <c r="J54" s="21"/>
       <c r="K54" s="21"/>
       <c r="L54" s="66"/>
       <c r="M54" s="66"/>
       <c r="N54" s="66"/>
       <c r="O54" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P54" s="22"/>
       <c r="Q54" s="22"/>
       <c r="R54" s="23"/>
       <c r="S54" s="15"/>
     </row>
-    <row r="55" spans="1:19" ht="30">
+    <row r="55" spans="1:19" ht="15">
       <c r="A55" s="19">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B55" s="92" t="s">
-        <v>72</v>
+        <v>5</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="D55" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E55" s="21"/>
-      <c r="F55" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="G55" s="73" t="s">
-        <v>73</v>
-      </c>
-      <c r="H55" s="73"/>
-      <c r="I55" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="J55" s="21"/>
+        <v>19</v>
+      </c>
+      <c r="D55" s="21"/>
+      <c r="E55" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="F55" s="21"/>
+      <c r="G55" s="74"/>
+      <c r="H55" s="74"/>
+      <c r="I55" s="74"/>
+      <c r="J55" s="21" t="s">
+        <v>80</v>
+      </c>
       <c r="K55" s="21"/>
-      <c r="L55" s="66" t="s">
-        <v>44</v>
-      </c>
+      <c r="L55" s="66"/>
       <c r="M55" s="66"/>
-      <c r="N55" s="66" t="s">
-        <v>44</v>
-      </c>
+      <c r="N55" s="66"/>
       <c r="O55" s="21" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="P55" s="22"/>
       <c r="Q55" s="22"/>
       <c r="R55" s="23"/>
       <c r="S55" s="15"/>
     </row>
-    <row r="56" spans="1:19">
+    <row r="56" spans="1:19" ht="30">
       <c r="A56" s="19">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B56" s="92" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="73"/>
+      <c r="F56" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G56" s="73" t="s">
+        <v>73</v>
+      </c>
       <c r="H56" s="73"/>
-      <c r="I56" s="69"/>
+      <c r="I56" s="69" t="s">
+        <v>93</v>
+      </c>
       <c r="J56" s="21"/>
       <c r="K56" s="21"/>
       <c r="L56" s="66" t="s">
@@ -3089,7 +3085,7 @@
         <v>44</v>
       </c>
       <c r="O56" s="21" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="P56" s="22"/>
       <c r="Q56" s="22"/>
@@ -3097,40 +3093,71 @@
       <c r="S56" s="15"/>
     </row>
     <row r="57" spans="1:19">
-      <c r="A57" s="86"/>
-      <c r="B57" s="87"/>
-      <c r="C57" s="88"/>
-      <c r="D57" s="88"/>
-      <c r="E57" s="88"/>
-      <c r="F57" s="88"/>
-      <c r="G57" s="94"/>
-      <c r="H57" s="95"/>
-      <c r="I57" s="95"/>
-      <c r="J57" s="88"/>
-      <c r="K57" s="88"/>
-      <c r="L57" s="89"/>
-      <c r="M57" s="89"/>
-      <c r="N57" s="89"/>
-      <c r="O57" s="88"/>
-      <c r="P57" s="90"/>
-      <c r="Q57" s="90"/>
-      <c r="R57" s="91"/>
+      <c r="A57" s="19">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B57" s="92" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="73"/>
+      <c r="H57" s="73"/>
+      <c r="I57" s="69"/>
+      <c r="J57" s="21"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="M57" s="66"/>
+      <c r="N57" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="O57" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="P57" s="22"/>
+      <c r="Q57" s="22"/>
+      <c r="R57" s="23"/>
       <c r="S57" s="15"/>
     </row>
     <row r="58" spans="1:19">
-      <c r="G58" s="41"/>
-      <c r="H58" s="41"/>
-      <c r="I58" s="41"/>
+      <c r="A58" s="86"/>
+      <c r="B58" s="87"/>
+      <c r="C58" s="88"/>
+      <c r="D58" s="88"/>
+      <c r="E58" s="88"/>
+      <c r="F58" s="88"/>
+      <c r="G58" s="94"/>
+      <c r="H58" s="95"/>
+      <c r="I58" s="95"/>
+      <c r="J58" s="88"/>
+      <c r="K58" s="88"/>
+      <c r="L58" s="89"/>
+      <c r="M58" s="89"/>
+      <c r="N58" s="89"/>
+      <c r="O58" s="88"/>
+      <c r="P58" s="90"/>
+      <c r="Q58" s="90"/>
+      <c r="R58" s="91"/>
+      <c r="S58" s="15"/>
     </row>
     <row r="59" spans="1:19">
-      <c r="G59" s="93"/>
-      <c r="H59" s="93"/>
-      <c r="I59" s="93"/>
+      <c r="G59" s="41"/>
+      <c r="H59" s="41"/>
+      <c r="I59" s="41"/>
     </row>
     <row r="60" spans="1:19">
-      <c r="G60" s="41"/>
-      <c r="H60" s="41"/>
-      <c r="I60" s="41"/>
+      <c r="G60" s="93"/>
+      <c r="H60" s="93"/>
+      <c r="I60" s="93"/>
     </row>
     <row r="61" spans="1:19">
       <c r="G61" s="41"/>
@@ -3157,34 +3184,39 @@
       <c r="H65" s="41"/>
       <c r="I65" s="41"/>
     </row>
+    <row r="66" spans="7:9">
+      <c r="G66" s="41"/>
+      <c r="H66" s="41"/>
+      <c r="I66" s="41"/>
+    </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
     <mergeCell ref="C11:F11"/>
-    <mergeCell ref="O48:P49"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="L48:L49"/>
-    <mergeCell ref="N48:N49"/>
-    <mergeCell ref="M48:M49"/>
-    <mergeCell ref="K48:K49"/>
-    <mergeCell ref="J48:J49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="H48:H49"/>
-    <mergeCell ref="I48:I49"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="O49:P50"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="L49:L50"/>
+    <mergeCell ref="N49:N50"/>
+    <mergeCell ref="M49:M50"/>
+    <mergeCell ref="K49:K50"/>
+    <mergeCell ref="J49:J50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="I49:I50"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F73 J73:N73" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F74 J74:N74" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3197,7 +3229,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15 K50:K57" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15 K51:K58" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>isAbstract</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{061A2328-C320-074B-A7A0-1D5ADA23E625}">
@@ -3219,7 +3251,7 @@
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>
           </x14:formula1>
-          <xm:sqref>L50:N57</xm:sqref>
+          <xm:sqref>L51:N58</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>